<commit_message>
Changed dates and added AE2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63F43E40-9F70-4DFA-BB47-9656E585E1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2207157D-DDD6-4F8F-8334-C5984240BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="151">
   <si>
     <t>week</t>
   </si>
@@ -99,15 +99,6 @@
     <t>Tu &amp; Th</t>
   </si>
   <si>
-    <t>Lab 00</t>
-  </si>
-  <si>
-    <t>/slides/lab-00.html</t>
-  </si>
-  <si>
-    <t>Waitlist disappears Friday</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -493,6 +484,9 @@
   </si>
   <si>
     <t>/hw/hw-00.html</t>
+  </si>
+  <si>
+    <t>/prepare/week-01.html</t>
   </si>
 </sst>
 </file>
@@ -1210,17 +1204,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1258,7 +1252,7 @@
     </row>
     <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1280,12 +1274,12 @@
         <v>14</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="33">
@@ -1299,7 +1293,9 @@
       <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1313,162 +1309,166 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5">
-      <c r="B4" s="10"/>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7" t="s">
+    <row r="4" spans="1:12" ht="66">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="6">
+        <v>45539</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" ht="66">
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45541</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="66">
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6">
-        <v>45539</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="66">
+      <c r="L5" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="49.5">
       <c r="B6" s="10"/>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="6">
-        <v>45541</v>
-      </c>
+      <c r="C6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="49.5">
-      <c r="B7" s="10"/>
-      <c r="C7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8"/>
+    <row r="7" spans="1:12" ht="99">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45546</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="G7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="K7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="99">
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
+      <c r="B8" s="10"/>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D8" s="6">
-        <v>45546</v>
+        <v>45548</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="J8" s="8"/>
-      <c r="K8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="8"/>
+      <c r="K8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="99">
       <c r="B9" s="10"/>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6">
-        <v>45548</v>
-      </c>
+      <c r="C9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="K9" s="8"/>
       <c r="L9" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="99">
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="8"/>
+    <row r="10" spans="1:12" ht="115.5">
+      <c r="B10" s="4">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45553</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1476,208 +1476,200 @@
       <c r="G10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="66">
+      <c r="B11" s="10"/>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6">
+        <v>45555</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="115.5">
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="6">
-        <v>45553</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="66">
+    <row r="12" spans="1:12" ht="16.5">
       <c r="B12" s="10"/>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6">
-        <v>45555</v>
-      </c>
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="G12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="8"/>
+      <c r="L12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.5">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="8"/>
+    </row>
+    <row r="13" spans="1:12" ht="66">
+      <c r="B13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="6">
+        <v>45560</v>
+      </c>
       <c r="E13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="K13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="66">
-      <c r="B14" s="4">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="6">
-        <v>45560</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="25">
+        <v>45562</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" ht="66">
+      <c r="B15" s="22"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5">
+      <c r="B16" s="10"/>
+      <c r="C16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" ht="49.5">
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="6">
+        <v>45567</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" ht="66">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23" t="s">
+      <c r="J17" s="8"/>
+      <c r="K17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:12" ht="16.5">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="25">
-        <v>45562</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-    </row>
-    <row r="16" spans="1:12" ht="66">
-      <c r="B16" s="22"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="2:12" ht="16.5">
-      <c r="B17" s="10"/>
-      <c r="C17" s="9" t="s">
+      <c r="D18" s="6">
+        <v>45569</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="2:12" ht="66">
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="2:12" ht="49.5">
-      <c r="B18" s="4">
-        <v>6</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="6">
-        <v>45567</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" ht="16.5">
-      <c r="B19" s="10"/>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="6">
-        <v>45569</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1688,37 +1680,45 @@
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12" ht="66">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="8"/>
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="6">
+        <v>45574</v>
+      </c>
       <c r="E20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:12" ht="66">
-      <c r="B21" s="4">
-        <v>7</v>
-      </c>
+      <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D21" s="6">
-        <v>45574</v>
+        <v>45576</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>76</v>
@@ -1731,189 +1731,187 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="2:12" ht="66">
+    <row r="22" spans="2:12" ht="16.5">
       <c r="B22" s="10"/>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="6">
-        <v>45576</v>
-      </c>
+      <c r="C22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" s="13"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="2:12" ht="16.5">
-      <c r="B23" s="10"/>
-      <c r="C23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7" t="s">
+      <c r="L22" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="66">
+      <c r="B23" s="4">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="6">
+        <v>45581</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>81</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="9" t="s">
-        <v>82</v>
-      </c>
+      <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" ht="115.5">
+      <c r="B24" s="10"/>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45583</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" ht="66">
-      <c r="B24" s="4">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="6">
-        <v>45581</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="115.5">
+    <row r="25" spans="2:12" ht="66">
       <c r="B25" s="10"/>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="6">
-        <v>45583</v>
-      </c>
+      <c r="C25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="13"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="66">
-      <c r="B26" s="10"/>
-      <c r="C26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="8"/>
+    <row r="26" spans="2:12" ht="99">
+      <c r="B26" s="4">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="6">
+        <v>45588</v>
+      </c>
       <c r="E26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="99">
-      <c r="B27" s="4">
-        <v>9</v>
-      </c>
+    <row r="27" spans="2:12" ht="132">
+      <c r="B27" s="10"/>
       <c r="C27" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D27" s="6">
-        <v>45588</v>
+        <v>45590</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>88</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I27" s="13"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="132">
+    <row r="28" spans="2:12" ht="49.5">
       <c r="B28" s="10"/>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="2:12" ht="49.5">
+      <c r="B29" s="4">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45595</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="2:12" ht="66">
+      <c r="B30" s="10"/>
+      <c r="C30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="6">
-        <v>45590</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="2:12" ht="49.5">
-      <c r="B29" s="10"/>
-      <c r="C29" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="2:12" ht="49.5">
-      <c r="B30" s="4">
-        <v>10</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D30" s="6">
-        <v>45595</v>
+        <v>45597</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>97</v>
@@ -1927,131 +1925,131 @@
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="66">
+    <row r="31" spans="2:12" ht="99">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D31" s="6">
-        <v>45597</v>
+        <v>45598</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="5" t="s">
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="2:12" ht="115.5">
+      <c r="B32" s="4">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="6">
+        <v>45602</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="2:12" ht="99">
-      <c r="B32" s="10"/>
-      <c r="C32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="6">
-        <v>45598</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="115.5">
-      <c r="B33" s="4">
+    <row r="33" spans="2:12" ht="99">
+      <c r="B33" s="10"/>
+      <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D33" s="6">
-        <v>45602</v>
+        <v>45604</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="8"/>
+      <c r="I33" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
+      <c r="K33" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="2:12" ht="99">
+    <row r="34" spans="2:12" ht="49.5">
       <c r="B34" s="10"/>
-      <c r="C34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="6">
-        <v>45604</v>
-      </c>
+      <c r="C34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="8"/>
       <c r="E34" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I34" s="9" t="s">
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J34" s="8"/>
-      <c r="K34" s="9" t="s">
+    </row>
+    <row r="35" spans="2:12" ht="82.5">
+      <c r="B35" s="4">
+        <v>12</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="6">
+        <v>45609</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="2:12" ht="49.5">
-      <c r="B35" s="10"/>
-      <c r="C35" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="8"/>
+      <c r="G35" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="13"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="L35" s="8"/>
     </row>
     <row r="36" spans="2:12" ht="82.5">
-      <c r="B36" s="4">
-        <v>12</v>
-      </c>
+      <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D36" s="6">
-        <v>45609</v>
+        <v>45611</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>114</v>
@@ -2065,88 +2063,82 @@
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="K36" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="L36" s="8"/>
     </row>
     <row r="37" spans="2:12" ht="82.5">
       <c r="B37" s="10"/>
-      <c r="C37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="6">
-        <v>45611</v>
-      </c>
+      <c r="C37" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="8"/>
       <c r="E37" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I37" s="13"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="13"/>
+      <c r="L37" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="2:12" ht="82.5">
-      <c r="B38" s="10"/>
-      <c r="C38" s="9" t="s">
+    </row>
+    <row r="38" spans="2:12" ht="33">
+      <c r="B38" s="4">
+        <v>13</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="6">
+        <v>45616</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="I38" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="12" t="s">
+      <c r="K38" s="9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" ht="33">
-      <c r="B39" s="4">
-        <v>13</v>
-      </c>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="2:12" ht="99">
+      <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D39" s="6">
-        <v>45616</v>
-      </c>
-      <c r="E39" s="7" t="s">
+        <v>45618</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>124</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="2:12" ht="82.5">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="2:12" ht="99">
-      <c r="B40" s="10"/>
-      <c r="C40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="6">
-        <v>45618</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -2156,125 +2148,127 @@
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="82.5">
-      <c r="B41" s="10"/>
-      <c r="C41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="11" t="s">
+    <row r="41" spans="2:12" ht="148.5">
+      <c r="B41" s="4">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45623</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="2:12" ht="148.5">
-      <c r="B42" s="4">
-        <v>14</v>
-      </c>
+      <c r="L41" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="49.5">
+      <c r="B42" s="10"/>
       <c r="C42" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D42" s="6">
-        <v>45623</v>
+        <v>45625</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="8"/>
+      <c r="G42" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I42" s="13"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="5" t="s">
-        <v>132</v>
-      </c>
+      <c r="K42" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L42" s="8"/>
     </row>
     <row r="43" spans="2:12" ht="49.5">
       <c r="B43" s="10"/>
-      <c r="C43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="6">
-        <v>45625</v>
-      </c>
+      <c r="C43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="7" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F43" s="8"/>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="2:12" ht="82.5">
+      <c r="B44" s="10"/>
+      <c r="C44" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="D44" s="6">
+        <v>45627</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="I43" s="13"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="2:12" ht="49.5">
-      <c r="B44" s="10"/>
-      <c r="C44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
+      <c r="J44" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K44" s="13"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="82.5">
-      <c r="B45" s="10"/>
+    <row r="45" spans="2:12" ht="16.5">
+      <c r="B45" s="4">
+        <v>15</v>
+      </c>
       <c r="C45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="6">
+        <v>45630</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D45" s="6">
-        <v>45627</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="K45" s="13"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="16.5">
-      <c r="B46" s="4">
-        <v>15</v>
-      </c>
+    <row r="46" spans="2:12" ht="99">
+      <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D46" s="6">
-        <v>45630</v>
+        <v>45632</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2282,35 +2276,37 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-    </row>
-    <row r="47" spans="2:12" ht="99">
+      <c r="L46" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="66">
       <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="6">
-        <v>45632</v>
-      </c>
+      <c r="C47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="8"/>
       <c r="E47" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="5" t="s">
+      <c r="J47" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="2:12" ht="132">
+      <c r="B48" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" ht="66">
-      <c r="B48" s="10"/>
-      <c r="C48" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="6">
+        <v>45639</v>
+      </c>
       <c r="E48" s="7" t="s">
         <v>143</v>
       </c>
@@ -2321,48 +2317,27 @@
       <c r="J48" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="K48" s="13"/>
-      <c r="L48" s="8"/>
-    </row>
-    <row r="49" spans="2:12" ht="132">
-      <c r="B49" s="4" t="s">
+      <c r="K48" s="8"/>
+      <c r="L48" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="6">
-        <v>45639</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="K49" s="8"/>
-      <c r="L49" s="5" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J48" r:id="rId1" location="presentation" display="https://sta210-fa23.netlify.app/project-instructions - presentation" xr:uid="{07C58870-EA52-4D63-AF17-B1B424283F9D}"/>
-    <hyperlink ref="J49" r:id="rId2" location="written-report" display="https://sta210-fa23.netlify.app/project-instructions - written-report" xr:uid="{3F2ABE08-AF15-4C8A-BD3B-2C483E2F4919}"/>
+    <hyperlink ref="J47" r:id="rId1" location="presentation" display="https://sta210-fa23.netlify.app/project-instructions - presentation" xr:uid="{07C58870-EA52-4D63-AF17-B1B424283F9D}"/>
+    <hyperlink ref="J48" r:id="rId2" location="written-report" display="https://sta210-fa23.netlify.app/project-instructions - written-report" xr:uid="{3F2ABE08-AF15-4C8A-BD3B-2C483E2F4919}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove navbar from cheatsheet
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2207157D-DDD6-4F8F-8334-C5984240BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B2513-B84B-41F6-AFF4-B7605B6B7DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="151">
   <si>
     <t>week</t>
   </si>
@@ -93,9 +93,6 @@
     <t>/ae/ae-02-bikeshare.html</t>
   </si>
   <si>
-    <t>Reproducibility + Mutlivariable relationships</t>
-  </si>
-  <si>
     <t>Tu &amp; Th</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>/prepare/week-01.html</t>
+  </si>
+  <si>
+    <t>RStudio + Mutlivariable relationships</t>
   </si>
 </sst>
 </file>
@@ -1207,14 +1207,14 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1274,15 +1274,18 @@
         <v>14</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="33">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
         <v>15</v>
@@ -1294,7 +1297,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
@@ -1306,7 +1309,7 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="66">
@@ -1314,13 +1317,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6">
         <v>45539</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1339,43 +1342,43 @@
         <v>45541</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="49.5">
       <c r="B6" s="10"/>
       <c r="C6" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="99">
@@ -1383,27 +1386,27 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <v>45546</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="8"/>
     </row>
@@ -1416,47 +1419,47 @@
         <v>45548</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="99">
       <c r="B9" s="10"/>
       <c r="C9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="115.5">
@@ -1464,17 +1467,17 @@
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
         <v>45553</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="8"/>
@@ -1491,43 +1494,43 @@
         <v>45555</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="I11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="16.5">
       <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="66">
@@ -1535,27 +1538,27 @@
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6">
         <v>45560</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" s="8"/>
     </row>
@@ -1568,11 +1571,11 @@
         <v>45562</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="27"/>
@@ -1585,7 +1588,7 @@
       <c r="C15" s="24"/>
       <c r="D15" s="26"/>
       <c r="E15" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="30"/>
@@ -1598,15 +1601,15 @@
     <row r="16" spans="1:12" ht="16.5">
       <c r="B16" s="10"/>
       <c r="C16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1619,27 +1622,27 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="6">
         <v>45567</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="I17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L17" s="8"/>
     </row>
@@ -1652,7 +1655,7 @@
         <v>45569</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1665,11 +1668,11 @@
     <row r="19" spans="2:12" ht="66">
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1684,22 +1687,22 @@
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="6">
         <v>45574</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
@@ -1715,16 +1718,16 @@
         <v>45576</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="H21" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="8"/>
@@ -1734,22 +1737,22 @@
     <row r="22" spans="2:12" ht="16.5">
       <c r="B22" s="10"/>
       <c r="C22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="66">
@@ -1757,13 +1760,13 @@
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="6">
         <v>45581</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -1782,11 +1785,11 @@
         <v>45583</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="8"/>
@@ -1797,11 +1800,11 @@
     <row r="25" spans="2:12" ht="66">
       <c r="B25" s="10"/>
       <c r="C25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -1816,20 +1819,20 @@
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="6">
         <v>45588</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="8"/>
@@ -1845,37 +1848,37 @@
         <v>45590</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L27" s="8"/>
     </row>
     <row r="28" spans="2:12" ht="49.5">
       <c r="B28" s="10"/>
       <c r="C28" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K28" s="13"/>
       <c r="L28" s="8"/>
@@ -1885,20 +1888,20 @@
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" s="6">
         <v>45595</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -1914,32 +1917,32 @@
         <v>45597</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L30" s="8"/>
     </row>
     <row r="31" spans="2:12" ht="99">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="6">
         <v>45598</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -1954,17 +1957,17 @@
         <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="6">
         <v>45602</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="8"/>
@@ -1981,32 +1984,32 @@
         <v>45604</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L33" s="8"/>
     </row>
     <row r="34" spans="2:12" ht="49.5">
       <c r="B34" s="10"/>
       <c r="C34" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -2015,7 +2018,7 @@
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="82.5">
@@ -2023,20 +2026,20 @@
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="6">
         <v>45609</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="8"/>
@@ -2052,30 +2055,30 @@
         <v>45611</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="8"/>
       <c r="K36" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L36" s="8"/>
     </row>
     <row r="37" spans="2:12" ht="82.5">
       <c r="B37" s="10"/>
       <c r="C37" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -2084,7 +2087,7 @@
       <c r="J37" s="8"/>
       <c r="K37" s="13"/>
       <c r="L37" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="33">
@@ -2092,23 +2095,23 @@
         <v>13</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" s="6">
         <v>45616</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L38" s="8"/>
     </row>
@@ -2121,7 +2124,7 @@
         <v>45618</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -2134,11 +2137,11 @@
     <row r="40" spans="2:12" ht="82.5">
       <c r="B40" s="10"/>
       <c r="C40" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -2153,26 +2156,26 @@
         <v>14</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="6">
         <v>45623</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="49.5">
@@ -2184,30 +2187,30 @@
         <v>45625</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="8"/>
       <c r="K42" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L42" s="8"/>
     </row>
     <row r="43" spans="2:12" ht="49.5">
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -2220,20 +2223,20 @@
     <row r="44" spans="2:12" ht="82.5">
       <c r="B44" s="10"/>
       <c r="C44" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" s="6">
         <v>45627</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K44" s="13"/>
       <c r="L44" s="8"/>
@@ -2243,13 +2246,13 @@
         <v>15</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" s="6">
         <v>45630</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2268,7 +2271,7 @@
         <v>45632</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2277,49 +2280,49 @@
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="66">
       <c r="B47" s="10"/>
       <c r="C47" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K47" s="13"/>
       <c r="L47" s="8"/>
     </row>
     <row r="48" spans="2:12" ht="132">
       <c r="B48" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="6">
         <v>45639</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K48" s="8"/>
       <c r="L48" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearraged a bunch of stuff
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{B79B2513-B84B-41F6-AFF4-B7605B6B7DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F1CD6B1-8238-45F1-B7A0-4C78D67ABB1D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECB6A89-F61B-4212-A3A4-B6B75194353A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="148">
   <si>
     <t>week</t>
   </si>
@@ -90,9 +90,6 @@
     <t>/slides/02-big-picture.html</t>
   </si>
   <si>
-    <t>/ae/ae-02-bikeshare.html</t>
-  </si>
-  <si>
     <t>Tu &amp; Th</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>/prepare/week-02.html</t>
   </si>
   <si>
-    <t>/slides/03-slr-intro.html</t>
-  </si>
-  <si>
     <t>/ae/ae-03-slr.html</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>/slides/04-slr-bootstrap.html</t>
   </si>
   <si>
-    <t>/ae/ae-04-bootstrap.html</t>
-  </si>
-  <si>
     <t>Statistics Experience assigned</t>
   </si>
   <si>
@@ -475,6 +466,18 @@
   </si>
   <si>
     <t>RStudio + Mutlivariable relationships</t>
+  </si>
+  <si>
+    <t>Multivariate Relationships</t>
+  </si>
+  <si>
+    <t>/slides/03-multivariate-relationship.html</t>
+  </si>
+  <si>
+    <t>/slides/04-slr-intro.html</t>
+  </si>
+  <si>
+    <t>HW 00 Due</t>
   </si>
 </sst>
 </file>
@@ -826,44 +829,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1204,14 +1207,14 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1247,9 +1250,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="16.5">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1268,17 +1271,17 @@
         <v>13</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="33">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16.5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
@@ -1291,105 +1294,104 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="66">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.5">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6">
         <v>45530</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>22</v>
+      <c r="E4" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66">
+    <row r="5" spans="1:12" ht="16.5">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="6">
-        <v>45541</v>
+        <v>45532</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="L5" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="99">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5">
       <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>45546</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="H6" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" ht="99">
+    <row r="7" spans="1:12" ht="16.5">
       <c r="B7" s="10"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
@@ -1398,65 +1400,65 @@
         <v>45548</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="I7" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="99">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16.5">
       <c r="B8" s="10"/>
       <c r="C8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="115.5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.5">
       <c r="B9" s="4">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6">
         <v>45553</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="8"/>
@@ -1464,7 +1466,7 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" ht="66">
+    <row r="10" spans="1:12" ht="16.5">
       <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>11</v>
@@ -1473,122 +1475,122 @@
         <v>45555</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" ht="16.5">
       <c r="B11" s="10"/>
       <c r="C11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="66">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16.5">
       <c r="B12" s="4">
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="6">
         <v>45560</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" ht="16.5">
+      <c r="B13" s="21"/>
+      <c r="C13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="25">
+        <v>45562</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="66">
-      <c r="B13" s="24"/>
-      <c r="C13" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="28">
-        <v>45562</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="1:12" ht="66">
-      <c r="B14" s="25"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.5">
+      <c r="B14" s="22"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:12" ht="16.5">
       <c r="B15" s="10"/>
       <c r="C15" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1596,32 +1598,32 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="33">
+    <row r="16" spans="1:12" ht="16.5">
       <c r="B16" s="4">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6">
         <v>45567</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L16" s="8"/>
     </row>
@@ -1634,7 +1636,7 @@
         <v>45569</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -1644,14 +1646,14 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="66">
+    <row r="18" spans="2:12" ht="16.5">
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1661,34 +1663,34 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="66">
+    <row r="19" spans="2:12" ht="16.5">
       <c r="B19" s="4">
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="6">
         <v>45574</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="66">
+    <row r="20" spans="2:12" ht="16.5">
       <c r="B20" s="10"/>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -1697,16 +1699,16 @@
         <v>45576</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
@@ -1716,36 +1718,36 @@
     <row r="21" spans="2:12" ht="16.5">
       <c r="B21" s="10"/>
       <c r="C21" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="66">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="16.5">
       <c r="B22" s="4">
         <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="6">
         <v>45581</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -1755,7 +1757,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="2:12" ht="115.5">
+    <row r="23" spans="2:12" ht="16.5">
       <c r="B23" s="10"/>
       <c r="C23" s="5" t="s">
         <v>11</v>
@@ -1764,11 +1766,11 @@
         <v>45583</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="8"/>
@@ -1776,14 +1778,14 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="66">
+    <row r="24" spans="2:12" ht="16.5">
       <c r="B24" s="10"/>
       <c r="C24" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -1793,32 +1795,32 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="99">
+    <row r="25" spans="2:12" ht="16.5">
       <c r="B25" s="4">
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="6">
         <v>45588</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="132">
+    <row r="26" spans="2:12" ht="16.5">
       <c r="B26" s="10"/>
       <c r="C26" s="5" t="s">
         <v>11</v>
@@ -1827,67 +1829,67 @@
         <v>45590</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="49.5">
+    <row r="27" spans="2:12" ht="16.5">
       <c r="B27" s="10"/>
       <c r="C27" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="49.5">
+    <row r="28" spans="2:12" ht="16.5">
       <c r="B28" s="4">
         <v>10</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="6">
         <v>45595</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="66">
+    <row r="29" spans="2:12" ht="16.5">
       <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
         <v>11</v>
@@ -1896,32 +1898,32 @@
         <v>45597</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="99">
+    <row r="30" spans="2:12" ht="16.5">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="6">
         <v>45598</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -1931,22 +1933,22 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="115.5">
+    <row r="31" spans="2:12" ht="16.5">
       <c r="B31" s="4">
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="6">
         <v>45602</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="8"/>
@@ -1954,7 +1956,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="99">
+    <row r="32" spans="2:12" ht="16.5">
       <c r="B32" s="10"/>
       <c r="C32" s="5" t="s">
         <v>11</v>
@@ -1963,32 +1965,32 @@
         <v>45604</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="49.5">
+    <row r="33" spans="2:12" ht="16.5">
       <c r="B33" s="10"/>
       <c r="C33" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -1997,35 +1999,35 @@
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="82.5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="16.5">
       <c r="B34" s="4">
         <v>12</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="6">
         <v>45609</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="82.5">
+    <row r="35" spans="2:12" ht="16.5">
       <c r="B35" s="10"/>
       <c r="C35" s="5" t="s">
         <v>11</v>
@@ -2034,30 +2036,30 @@
         <v>45611</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="8"/>
       <c r="K35" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5">
+    <row r="36" spans="2:12" ht="16.5">
       <c r="B36" s="10"/>
       <c r="C36" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
@@ -2066,35 +2068,35 @@
       <c r="J36" s="8"/>
       <c r="K36" s="13"/>
       <c r="L36" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="33">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="16.5">
       <c r="B37" s="4">
         <v>13</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="6">
         <v>45616</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="99">
+    <row r="38" spans="2:12" ht="16.5">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>11</v>
@@ -2103,7 +2105,7 @@
         <v>45618</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -2113,14 +2115,14 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="66">
+    <row r="39" spans="2:12" ht="16.5">
       <c r="B39" s="10"/>
       <c r="C39" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -2130,34 +2132,34 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="148.5">
+    <row r="40" spans="2:12" ht="16.5">
       <c r="B40" s="4">
         <v>14</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="6">
         <v>45623</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" ht="33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="16.5">
       <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
         <v>11</v>
@@ -2166,30 +2168,30 @@
         <v>45625</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="8"/>
       <c r="K41" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="2:12" ht="49.5">
+    <row r="42" spans="2:12" ht="16.5">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -2199,23 +2201,23 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="82.5">
+    <row r="43" spans="2:12" ht="16.5">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D43" s="6">
         <v>45627</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K43" s="13"/>
       <c r="L43" s="8"/>
@@ -2225,13 +2227,13 @@
         <v>15</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="6">
         <v>45630</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -2241,7 +2243,7 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="99">
+    <row r="45" spans="2:12" ht="16.5">
       <c r="B45" s="10"/>
       <c r="C45" s="5" t="s">
         <v>11</v>
@@ -2250,7 +2252,7 @@
         <v>45632</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2259,69 +2261,53 @@
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="66">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="16.5">
       <c r="B46" s="10"/>
       <c r="C46" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K46" s="13"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="115.5">
+    <row r="47" spans="2:12" ht="16.5">
       <c r="B47" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="6">
         <v>45639</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="H13:H14"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="J46" r:id="rId1" location="presentation" display="https://sta210-fa23.netlify.app/project-instructions - presentation" xr:uid="{07C58870-EA52-4D63-AF17-B1B424283F9D}"/>
-    <hyperlink ref="J47" r:id="rId2" location="written-report" display="https://sta210-fa23.netlify.app/project-instructions - written-report" xr:uid="{3F2ABE08-AF15-4C8A-BD3B-2C483E2F4919}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated lecture 3 link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECB6A89-F61B-4212-A3A4-B6B75194353A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A4C096-5863-4A2F-B360-CC768A6EC37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -471,13 +471,13 @@
     <t>Multivariate Relationships</t>
   </si>
   <si>
-    <t>/slides/03-multivariate-relationship.html</t>
-  </si>
-  <si>
     <t>/slides/04-slr-intro.html</t>
   </si>
   <si>
     <t>HW 00 Due</t>
+  </si>
+  <si>
+    <t>/slides/03-multivariate-relationships.html</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1207,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1250,7 +1250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.5">
+    <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5">
+    <row r="3" spans="1:12" ht="33">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5">
+    <row r="4" spans="1:12" ht="66">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -1323,14 +1323,14 @@
         <v>144</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="16.5">
+    <row r="5" spans="1:12" ht="66">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>14</v>
@@ -1356,13 +1356,13 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.5">
+    <row r="6" spans="1:12" ht="99">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5">
+    <row r="7" spans="1:12" ht="99">
       <c r="B7" s="10"/>
       <c r="C7" s="5" t="s">
         <v>11</v>
@@ -1422,7 +1422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.5">
+    <row r="8" spans="1:12" ht="99">
       <c r="B8" s="10"/>
       <c r="C8" s="9" t="s">
         <v>18</v>
@@ -1443,7 +1443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.5">
+    <row r="9" spans="1:12" ht="115.5">
       <c r="B9" s="4">
         <v>4</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" ht="16.5">
+    <row r="10" spans="1:12" ht="66">
       <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>11</v>
@@ -1514,7 +1514,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="66">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="66">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>11</v>
@@ -1564,7 +1564,7 @@
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5">
+    <row r="14" spans="1:12" ht="66">
       <c r="B14" s="22"/>
       <c r="C14" s="24"/>
       <c r="D14" s="26"/>
@@ -1598,7 +1598,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5">
+    <row r="16" spans="1:12" ht="33">
       <c r="B16" s="4">
         <v>6</v>
       </c>
@@ -1646,7 +1646,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="16.5">
+    <row r="18" spans="2:12" ht="66">
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
         <v>18</v>
@@ -1663,7 +1663,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="16.5">
+    <row r="19" spans="2:12" ht="66">
       <c r="B19" s="4">
         <v>7</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="16.5">
+    <row r="20" spans="2:12" ht="66">
       <c r="B20" s="10"/>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -1736,7 +1736,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="16.5">
+    <row r="22" spans="2:12" ht="66">
       <c r="B22" s="4">
         <v>8</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="2:12" ht="16.5">
+    <row r="23" spans="2:12" ht="115.5">
       <c r="B23" s="10"/>
       <c r="C23" s="5" t="s">
         <v>11</v>
@@ -1778,7 +1778,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="16.5">
+    <row r="24" spans="2:12" ht="66">
       <c r="B24" s="10"/>
       <c r="C24" s="9" t="s">
         <v>18</v>
@@ -1795,7 +1795,7 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="16.5">
+    <row r="25" spans="2:12" ht="99">
       <c r="B25" s="4">
         <v>9</v>
       </c>
@@ -1820,7 +1820,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="16.5">
+    <row r="26" spans="2:12" ht="132">
       <c r="B26" s="10"/>
       <c r="C26" s="5" t="s">
         <v>11</v>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="16.5">
+    <row r="27" spans="2:12" ht="49.5">
       <c r="B27" s="10"/>
       <c r="C27" s="9" t="s">
         <v>18</v>
@@ -1864,7 +1864,7 @@
       <c r="K27" s="13"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="16.5">
+    <row r="28" spans="2:12" ht="49.5">
       <c r="B28" s="4">
         <v>10</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="16.5">
+    <row r="29" spans="2:12" ht="66">
       <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
         <v>11</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="16.5">
+    <row r="30" spans="2:12" ht="99">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
         <v>18</v>
@@ -1933,7 +1933,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="16.5">
+    <row r="31" spans="2:12" ht="115.5">
       <c r="B31" s="4">
         <v>11</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="16.5">
+    <row r="32" spans="2:12" ht="99">
       <c r="B32" s="10"/>
       <c r="C32" s="5" t="s">
         <v>11</v>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="16.5">
+    <row r="33" spans="2:12" ht="49.5">
       <c r="B33" s="10"/>
       <c r="C33" s="9" t="s">
         <v>18</v>
@@ -2002,7 +2002,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="16.5">
+    <row r="34" spans="2:12" ht="82.5">
       <c r="B34" s="4">
         <v>12</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="16.5">
+    <row r="35" spans="2:12" ht="82.5">
       <c r="B35" s="10"/>
       <c r="C35" s="5" t="s">
         <v>11</v>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="16.5">
+    <row r="36" spans="2:12" ht="82.5">
       <c r="B36" s="10"/>
       <c r="C36" s="9" t="s">
         <v>110</v>
@@ -2071,7 +2071,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="16.5">
+    <row r="37" spans="2:12" ht="33">
       <c r="B37" s="4">
         <v>13</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="16.5">
+    <row r="38" spans="2:12" ht="99">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>11</v>
@@ -2115,7 +2115,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="16.5">
+    <row r="39" spans="2:12" ht="66">
       <c r="B39" s="10"/>
       <c r="C39" s="9" t="s">
         <v>18</v>
@@ -2132,7 +2132,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="16.5">
+    <row r="40" spans="2:12" ht="148.5">
       <c r="B40" s="4">
         <v>14</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="16.5">
+    <row r="41" spans="2:12" ht="33">
       <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
         <v>11</v>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="2:12" ht="16.5">
+    <row r="42" spans="2:12" ht="49.5">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
         <v>18</v>
@@ -2201,7 +2201,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="16.5">
+    <row r="43" spans="2:12" ht="82.5">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
         <v>126</v>
@@ -2243,7 +2243,7 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="16.5">
+    <row r="45" spans="2:12" ht="99">
       <c r="B45" s="10"/>
       <c r="C45" s="5" t="s">
         <v>11</v>
@@ -2264,7 +2264,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="16.5">
+    <row r="46" spans="2:12" ht="66">
       <c r="B46" s="10"/>
       <c r="C46" s="9" t="s">
         <v>18</v>
@@ -2283,7 +2283,7 @@
       <c r="K46" s="13"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="16.5">
+    <row r="47" spans="2:12" ht="115.5">
       <c r="B47" s="4" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Updated schedule and AE2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A4C096-5863-4A2F-B360-CC768A6EC37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE898A3-6D0B-4BE9-9754-A0F7547B4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
   <si>
     <t>week</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>/slides/03-multivariate-relationships.html</t>
+  </si>
+  <si>
+    <t>SLR - Prediction</t>
+  </si>
+  <si>
+    <t>/slides/05-slr-prediction.html</t>
+  </si>
+  <si>
+    <t>/ae/ae-02-bikeshare.html</t>
   </si>
 </sst>
 </file>
@@ -577,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -766,13 +775,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -866,6 +888,9 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1204,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1362,298 +1387,307 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="99">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
+    <row r="6" spans="1:12" ht="49.5">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="6">
-        <v>45546</v>
+        <v>45534</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="33"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="99">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45546</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="99">
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6">
-        <v>45548</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="99">
       <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6">
+        <v>45548</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="99">
+      <c r="B9" s="10"/>
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="115.5">
-      <c r="B9" s="4">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6">
-        <v>45553</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="66">
-      <c r="B10" s="10"/>
+      <c r="L9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="115.5">
+      <c r="B10" s="4">
+        <v>4</v>
+      </c>
       <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45553</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="66">
+      <c r="B11" s="10"/>
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>45555</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="5" t="s">
+      <c r="J11" s="8"/>
+      <c r="K11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.5">
-      <c r="B11" s="10"/>
-      <c r="C11" s="9" t="s">
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="5" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="66">
-      <c r="B12" s="4">
+    <row r="13" spans="1:12" ht="66">
+      <c r="B13" s="4">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="6">
         <v>45560</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="9" t="s">
+      <c r="J13" s="8"/>
+      <c r="K13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="66">
-      <c r="B13" s="21"/>
-      <c r="C13" s="23" t="s">
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="66">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D14" s="25">
         <v>45562</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="29" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-    </row>
-    <row r="14" spans="1:12" ht="66">
-      <c r="B14" s="22"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="15" t="s">
+      <c r="H14" s="31"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" ht="66">
+      <c r="B15" s="22"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.5">
-      <c r="B15" s="10"/>
-      <c r="C15" s="9" t="s">
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5">
+      <c r="B16" s="10"/>
+      <c r="C16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="7" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" ht="33">
-      <c r="B16" s="4">
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" ht="33">
+      <c r="B17" s="4">
         <v>6</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="6">
         <v>45567</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="5" t="s">
+      <c r="J17" s="8"/>
+      <c r="K17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="2:12" ht="16.5">
-      <c r="B17" s="10"/>
-      <c r="C17" s="5" t="s">
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:12" ht="16.5">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <v>45569</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="2:12" ht="66">
-      <c r="B18" s="10"/>
-      <c r="C18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1664,465 +1698,465 @@
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="2:12" ht="66">
-      <c r="B19" s="4">
-        <v>7</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="6">
-        <v>45574</v>
-      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="13"/>
+        <v>62</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12" ht="66">
-      <c r="B20" s="10"/>
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
       <c r="C20" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6">
-        <v>45576</v>
+        <v>45574</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="16.5">
+    <row r="21" spans="2:12" ht="66">
       <c r="B21" s="10"/>
-      <c r="C21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="8"/>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="6">
+        <v>45576</v>
+      </c>
       <c r="E21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="13"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="66">
-      <c r="B22" s="4">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="6">
-        <v>45581</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>73</v>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="2:12" ht="16.5">
+      <c r="B22" s="10"/>
+      <c r="C22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="2:12" ht="115.5">
-      <c r="B23" s="10"/>
+      <c r="L22" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="66">
+      <c r="B23" s="4">
+        <v>8</v>
+      </c>
       <c r="C23" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D23" s="6">
-        <v>45583</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>45581</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="13"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="66">
+    <row r="24" spans="2:12" ht="115.5">
       <c r="B24" s="10"/>
-      <c r="C24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="8"/>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45583</v>
+      </c>
       <c r="E24" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="13"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="99">
-      <c r="B25" s="4">
-        <v>9</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="6">
-        <v>45588</v>
-      </c>
+    <row r="25" spans="2:12" ht="66">
+      <c r="B25" s="10"/>
+      <c r="C25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="13"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="132">
-      <c r="B26" s="10"/>
+    <row r="26" spans="2:12" ht="99">
+      <c r="B26" s="4">
+        <v>9</v>
+      </c>
       <c r="C26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="6">
+        <v>45588</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="2:12" ht="132">
+      <c r="B27" s="10"/>
+      <c r="C27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>45590</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="9" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="9" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="9" t="s">
+      <c r="J27" s="8"/>
+      <c r="K27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="2:12" ht="49.5">
-      <c r="B27" s="10"/>
-      <c r="C27" s="9" t="s">
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="2:12" ht="49.5">
+      <c r="B28" s="10"/>
+      <c r="C28" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="7" t="s">
+      <c r="D28" s="8"/>
+      <c r="E28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="9" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="2:12" ht="49.5">
-      <c r="B28" s="4">
+      <c r="K28" s="13"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="2:12" ht="49.5">
+      <c r="B29" s="4">
         <v>10</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>45595</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="2:12" ht="66">
-      <c r="B29" s="10"/>
-      <c r="C29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="6">
-        <v>45597</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="K29" s="8"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="99">
+    <row r="30" spans="2:12" ht="66">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D30" s="6">
-        <v>45598</v>
+        <v>45597</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="G30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="115.5">
-      <c r="B31" s="4">
-        <v>11</v>
-      </c>
+    <row r="31" spans="2:12" ht="99">
+      <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="6">
-        <v>45602</v>
+        <v>45598</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H31" s="13"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="99">
-      <c r="B32" s="10"/>
+    <row r="32" spans="2:12" ht="115.5">
+      <c r="B32" s="4">
+        <v>11</v>
+      </c>
       <c r="C32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="6">
+        <v>45602</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="2:12" ht="99">
+      <c r="B33" s="10"/>
+      <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <v>45604</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="5" t="s">
+      <c r="F33" s="8"/>
+      <c r="G33" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J32" s="8"/>
-      <c r="K32" s="9" t="s">
+      <c r="J33" s="8"/>
+      <c r="K33" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="2:12" ht="49.5">
-      <c r="B33" s="10"/>
-      <c r="C33" s="9" t="s">
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="2:12" ht="49.5">
+      <c r="B34" s="10"/>
+      <c r="C34" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7" t="s">
+      <c r="D34" s="8"/>
+      <c r="E34" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="82.5">
-      <c r="B34" s="4">
-        <v>12</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="6">
-        <v>45609</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I34" s="13"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
+      <c r="L34" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="35" spans="2:12" ht="82.5">
-      <c r="B35" s="10"/>
+      <c r="B35" s="4">
+        <v>12</v>
+      </c>
       <c r="C35" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D35" s="6">
-        <v>45611</v>
+        <v>45609</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="16" t="s">
-        <v>109</v>
-      </c>
+      <c r="K35" s="8"/>
       <c r="L35" s="8"/>
     </row>
     <row r="36" spans="2:12" ht="82.5">
       <c r="B36" s="10"/>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45611</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="2:12" ht="82.5">
+      <c r="B37" s="10"/>
+      <c r="C37" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="7" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="33">
-      <c r="B37" s="4">
-        <v>13</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="6">
-        <v>45616</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="9" t="s">
-        <v>114</v>
-      </c>
+      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="2:12" ht="99">
-      <c r="B38" s="10"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="33">
+      <c r="B38" s="4">
+        <v>13</v>
+      </c>
       <c r="C38" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D38" s="6">
-        <v>45618</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>116</v>
+        <v>45616</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="I38" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
+      <c r="K38" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="66">
+    <row r="39" spans="2:12" ht="99">
       <c r="B39" s="10"/>
-      <c r="C39" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="8"/>
+      <c r="C39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="6">
+        <v>45618</v>
+      </c>
       <c r="E39" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -2132,127 +2166,125 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="148.5">
-      <c r="B40" s="4">
-        <v>14</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="6">
-        <v>45623</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H40" s="13"/>
+    <row r="40" spans="2:12" ht="66">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="5" t="s">
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="2:12" ht="148.5">
+      <c r="B41" s="4">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45623</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H41" s="13"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="33">
-      <c r="B41" s="10"/>
-      <c r="C41" s="5" t="s">
+    <row r="42" spans="2:12" ht="33">
+      <c r="B42" s="10"/>
+      <c r="C42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <v>45625</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E42" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="5" t="s">
+      <c r="F42" s="8"/>
+      <c r="G42" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="I41" s="13"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="5" t="s">
+      <c r="I42" s="13"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="2:12" ht="49.5">
-      <c r="B42" s="10"/>
-      <c r="C42" s="9" t="s">
+      <c r="L42" s="8"/>
+    </row>
+    <row r="43" spans="2:12" ht="49.5">
+      <c r="B43" s="10"/>
+      <c r="C43" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="7" t="s">
+      <c r="D43" s="8"/>
+      <c r="E43" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="2:12" ht="82.5">
-      <c r="B43" s="10"/>
-      <c r="C43" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D43" s="6">
-        <v>45627</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
-      <c r="J43" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="K43" s="13"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="16.5">
-      <c r="B44" s="4">
-        <v>15</v>
-      </c>
+    <row r="44" spans="2:12" ht="82.5">
+      <c r="B44" s="10"/>
       <c r="C44" s="5" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="D44" s="6">
-        <v>45630</v>
+        <v>45627</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
+      <c r="J44" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K44" s="13"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="99">
-      <c r="B45" s="10"/>
+    <row r="45" spans="2:12" ht="16.5">
+      <c r="B45" s="4">
+        <v>15</v>
+      </c>
       <c r="C45" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D45" s="6">
-        <v>45632</v>
+        <v>45630</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2260,49 +2292,68 @@
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
-      <c r="L45" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="66">
+      <c r="L45" s="8"/>
+    </row>
+    <row r="46" spans="2:12" ht="99">
       <c r="B46" s="10"/>
-      <c r="C46" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="8"/>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="6">
+        <v>45632</v>
+      </c>
       <c r="E46" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
-      <c r="J46" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="K46" s="13"/>
-      <c r="L46" s="8"/>
-    </row>
-    <row r="47" spans="2:12" ht="115.5">
-      <c r="B47" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="6">
-        <v>45639</v>
-      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="66">
+      <c r="B47" s="10"/>
+      <c r="C47" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="8"/>
       <c r="E47" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="2:12" ht="115.5">
+      <c r="B48" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="6">
+        <v>45639</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K47" s="8"/>
-      <c r="L47" s="5" t="s">
+      <c r="K48" s="8"/>
+      <c r="L48" s="5" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved hw1 due date
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CCC3F5-8D59-4BBC-AED1-B10EECE97831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{81CCC3F5-8D59-4BBC-AED1-B10EECE97831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5C83DED-5520-4434-94E3-E806E58558F4}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="147">
   <si>
     <t>week</t>
   </si>
@@ -115,15 +115,6 @@
   </si>
   <si>
     <t>Include prediction intervals</t>
-  </si>
-  <si>
-    <t>Lab 02: Ice duration and air temperature</t>
-  </si>
-  <si>
-    <t>/slides/lab-02.html</t>
-  </si>
-  <si>
-    <t>Individual lab</t>
   </si>
   <si>
     <t>SLR: Mathematical models for inference</t>
@@ -490,7 +481,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1237,17 +1228,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1283,9 +1274,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1304,17 +1295,17 @@
         <v>13</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="33">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
@@ -1327,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
@@ -1336,12 +1327,12 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="66">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -1353,19 +1344,19 @@
         <v>45530</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66">
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
@@ -1381,7 +1372,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>14</v>
@@ -1391,15 +1382,15 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5">
+    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
@@ -1409,23 +1400,23 @@
         <v>45534</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="33"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1437,12 +1428,12 @@
         <v>45537</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="99">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
@@ -1455,24 +1446,21 @@
         <v>23</v>
       </c>
       <c r="F8" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="165">
+    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
@@ -1482,30 +1470,36 @@
         <v>45541</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="99">
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8"/>
+    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45553</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1513,208 +1507,200 @@
       <c r="G10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6">
+        <v>45555</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="115.5">
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6">
-        <v>45553</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="66">
-      <c r="B12" s="10"/>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6">
-        <v>45555</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.5">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="6">
+        <v>45560</v>
+      </c>
       <c r="E13" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="66">
-      <c r="B14" s="4">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="K13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="25">
+        <v>45562</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="31"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="6">
-        <v>45560</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="D17" s="6">
+        <v>45567</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" ht="66">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23" t="s">
+      <c r="J17" s="8"/>
+      <c r="K17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="25">
-        <v>45562</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-    </row>
-    <row r="16" spans="1:12" ht="66">
-      <c r="B16" s="22"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="2:12" ht="16.5">
-      <c r="B17" s="10"/>
-      <c r="C17" s="9" t="s">
+      <c r="D18" s="6">
+        <v>45569</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="2:12" ht="33">
-      <c r="B18" s="4">
-        <v>6</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="6">
-        <v>45567</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" ht="16.5">
-      <c r="B19" s="10"/>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="6">
-        <v>45569</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1724,38 +1710,46 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="66">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="8"/>
+    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="6">
+        <v>45574</v>
+      </c>
       <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="66">
-      <c r="B21" s="4">
-        <v>7</v>
-      </c>
+    <row r="21" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D21" s="6">
-        <v>45574</v>
+        <v>45576</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>57</v>
@@ -1768,189 +1762,187 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="2:12" ht="66">
+    <row r="22" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="6">
-        <v>45576</v>
-      </c>
+      <c r="C22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I22" s="13"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="2:12" ht="16.5">
-      <c r="B23" s="10"/>
-      <c r="C23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7" t="s">
+      <c r="L22" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B23" s="4">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="6">
+        <v>45581</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45583</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" ht="66">
-      <c r="B24" s="4">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="6">
-        <v>45581</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="115.5">
+    <row r="25" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="6">
-        <v>45583</v>
-      </c>
+      <c r="C25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="13"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="66">
-      <c r="B26" s="10"/>
-      <c r="C26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="8"/>
+    <row r="26" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B26" s="4">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="6">
+        <v>45588</v>
+      </c>
       <c r="E26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="99">
-      <c r="B27" s="4">
-        <v>9</v>
-      </c>
+    <row r="27" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D27" s="6">
-        <v>45588</v>
+        <v>45590</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>69</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I27" s="13"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="132">
+    <row r="28" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="4">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45595</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="6">
-        <v>45590</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="2:12" ht="49.5">
-      <c r="B29" s="10"/>
-      <c r="C29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="2:12" ht="49.5">
-      <c r="B30" s="4">
-        <v>10</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D30" s="6">
-        <v>45595</v>
+        <v>45597</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>78</v>
@@ -1964,131 +1956,131 @@
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="66">
+    <row r="31" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D31" s="6">
-        <v>45597</v>
+        <v>45598</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="5" t="s">
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="4">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="6">
+        <v>45602</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="2:12" ht="99">
-      <c r="B32" s="10"/>
-      <c r="C32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="6">
-        <v>45598</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="115.5">
-      <c r="B33" s="4">
+    <row r="33" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B33" s="10"/>
+      <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="6">
+        <v>45604</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" s="8"/>
+      <c r="K33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B34" s="10"/>
+      <c r="C34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B35" s="4">
+        <v>12</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="6">
-        <v>45602</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="2:12" ht="99">
-      <c r="B34" s="10"/>
-      <c r="C34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="6">
-        <v>45604</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="J34" s="8"/>
-      <c r="K34" s="9" t="s">
+      <c r="D35" s="6">
+        <v>45609</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="2:12" ht="49.5">
-      <c r="B35" s="10"/>
-      <c r="C35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="8"/>
+      <c r="G35" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="13"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="82.5">
-      <c r="B36" s="4">
-        <v>12</v>
-      </c>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D36" s="6">
-        <v>45609</v>
+        <v>45611</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>95</v>
@@ -2102,88 +2094,82 @@
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="K36" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="2:12" ht="82.5">
+    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B37" s="10"/>
-      <c r="C37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="6">
-        <v>45611</v>
-      </c>
+      <c r="C37" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="8"/>
       <c r="E37" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I37" s="13"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="13"/>
+      <c r="L37" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="2:12" ht="82.5">
-      <c r="B38" s="10"/>
-      <c r="C38" s="9" t="s">
+    </row>
+    <row r="38" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B38" s="4">
+        <v>13</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="6">
+        <v>45616</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="I38" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="12" t="s">
+      <c r="K38" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" ht="33">
-      <c r="B39" s="4">
-        <v>13</v>
-      </c>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D39" s="6">
-        <v>45616</v>
-      </c>
-      <c r="E39" s="7" t="s">
+        <v>45618</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>105</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="2:12" ht="99">
-      <c r="B40" s="10"/>
-      <c r="C40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="6">
-        <v>45618</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -2193,125 +2179,127 @@
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="66">
-      <c r="B41" s="10"/>
-      <c r="C41" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="11" t="s">
+    <row r="41" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B41" s="4">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45623</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="2:12" ht="148.5">
-      <c r="B42" s="4">
-        <v>14</v>
-      </c>
+      <c r="L41" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
       <c r="C42" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D42" s="6">
-        <v>45623</v>
+        <v>45625</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="8"/>
+      <c r="G42" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="13"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" ht="33">
+      <c r="K42" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L42" s="8"/>
+    </row>
+    <row r="43" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
-      <c r="C43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="6">
-        <v>45625</v>
-      </c>
+      <c r="C43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="7" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F43" s="8"/>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B44" s="10"/>
+      <c r="C44" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="D44" s="6">
+        <v>45627</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="I43" s="13"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="2:12" ht="49.5">
-      <c r="B44" s="10"/>
-      <c r="C44" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
+      <c r="J44" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K44" s="13"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="82.5">
-      <c r="B45" s="10"/>
+    <row r="45" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B45" s="4">
+        <v>15</v>
+      </c>
       <c r="C45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="6">
+        <v>45630</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D45" s="6">
-        <v>45627</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="K45" s="13"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="16.5">
-      <c r="B46" s="4">
-        <v>15</v>
-      </c>
+    <row r="46" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D46" s="6">
-        <v>45630</v>
+        <v>45632</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2319,35 +2307,37 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-    </row>
-    <row r="47" spans="2:12" ht="99">
+      <c r="L46" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="6">
-        <v>45632</v>
-      </c>
+      <c r="C47" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="8"/>
       <c r="E47" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="5" t="s">
+      <c r="J47" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="2:12" ht="165" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" ht="66">
-      <c r="B48" s="10"/>
-      <c r="C48" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="6">
+        <v>45639</v>
+      </c>
       <c r="E48" s="7" t="s">
         <v>124</v>
       </c>
@@ -2358,30 +2348,9 @@
       <c r="J48" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="K48" s="13"/>
-      <c r="L48" s="8"/>
-    </row>
-    <row r="49" spans="2:12" ht="115.5">
-      <c r="B49" s="4" t="s">
+      <c r="K48" s="8"/>
+      <c r="L48" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="6">
-        <v>45639</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="K49" s="8"/>
-      <c r="L49" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added math models slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricF\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD9C87-EF71-4A9E-95D8-857D587B68BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD34FDC0-686A-46BA-91B4-5570855C0291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
   <si>
     <t>week</t>
   </si>
@@ -120,9 +120,6 @@
     <t>SLR: Mathematical models for inference</t>
   </si>
   <si>
-    <t>/slides/06-slr-math-models.html</t>
-  </si>
-  <si>
     <t>SLR: Model conditions</t>
   </si>
   <si>
@@ -481,13 +478,19 @@
   </si>
   <si>
     <t>/ae/ae-04-sim-testing.html</t>
+  </si>
+  <si>
+    <t>/prepare/math-models-prep.html</t>
+  </si>
+  <si>
+    <t>/slides/08-slr-math-models.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1236,15 +1239,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1280,9 +1283,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1301,17 +1304,17 @@
         <v>13</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="33">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
@@ -1324,7 +1327,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
@@ -1333,12 +1336,12 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="66">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -1350,19 +1353,19 @@
         <v>45530</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="66">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
@@ -1378,7 +1381,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>14</v>
@@ -1388,15 +1391,15 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="49.5">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
@@ -1406,23 +1409,23 @@
         <v>45534</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="33"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1434,12 +1437,12 @@
         <v>45537</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="99">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
@@ -1452,26 +1455,26 @@
         <v>23</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="165">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
@@ -1481,27 +1484,30 @@
         <v>45541</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
       <c r="K9" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="115.5">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
       <c r="B10" s="4">
         <v>4</v>
       </c>
@@ -1509,14 +1515,16 @@
         <v>19</v>
       </c>
       <c r="D10" s="6">
-        <v>45553</v>
+        <v>45544</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="G10" s="9" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="8"/>
@@ -1524,7 +1532,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="66">
       <c r="B11" s="10"/>
       <c r="C11" s="5" t="s">
         <v>11</v>
@@ -1533,46 +1541,46 @@
         <v>45555</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="16.5">
       <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="66">
       <c r="B13" s="4">
         <v>5</v>
       </c>
@@ -1583,25 +1591,25 @@
         <v>45560</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="66">
       <c r="B14" s="21"/>
       <c r="C14" s="23" t="s">
         <v>11</v>
@@ -1610,11 +1618,11 @@
         <v>45562</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="27"/>
@@ -1622,12 +1630,12 @@
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
     </row>
-    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="66">
       <c r="B15" s="22"/>
       <c r="C15" s="24"/>
       <c r="D15" s="26"/>
       <c r="E15" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="30"/>
@@ -1637,18 +1645,18 @@
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="16.5">
       <c r="B16" s="10"/>
       <c r="C16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1656,7 +1664,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="33">
       <c r="B17" s="4">
         <v>6</v>
       </c>
@@ -1667,25 +1675,25 @@
         <v>45567</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="I17" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="16.5">
       <c r="B18" s="10"/>
       <c r="C18" s="5" t="s">
         <v>11</v>
@@ -1694,7 +1702,7 @@
         <v>45569</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1704,14 +1712,14 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="66">
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1721,7 +1729,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="66">
       <c r="B20" s="4">
         <v>7</v>
       </c>
@@ -1732,23 +1740,23 @@
         <v>45574</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="66">
       <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
         <v>11</v>
@@ -1757,44 +1765,44 @@
         <v>45576</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="H21" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="16.5">
       <c r="B22" s="10"/>
       <c r="C22" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="66">
       <c r="B23" s="4">
         <v>8</v>
       </c>
@@ -1805,7 +1813,7 @@
         <v>45581</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -1815,7 +1823,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="115.5">
       <c r="B24" s="10"/>
       <c r="C24" s="5" t="s">
         <v>11</v>
@@ -1824,11 +1832,11 @@
         <v>45583</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="8"/>
@@ -1836,14 +1844,14 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="66">
       <c r="B25" s="10"/>
       <c r="C25" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -1853,7 +1861,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="99">
       <c r="B26" s="4">
         <v>9</v>
       </c>
@@ -1864,21 +1872,21 @@
         <v>45588</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="165" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="132">
       <c r="B27" s="10"/>
       <c r="C27" s="5" t="s">
         <v>11</v>
@@ -1887,42 +1895,42 @@
         <v>45590</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="49.5">
       <c r="B28" s="10"/>
       <c r="C28" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K28" s="13"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="49.5">
       <c r="B29" s="4">
         <v>10</v>
       </c>
@@ -1933,21 +1941,21 @@
         <v>45595</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" ht="66">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1956,23 +1964,23 @@
         <v>45597</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="132" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" ht="99">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
         <v>18</v>
@@ -1981,7 +1989,7 @@
         <v>45598</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -1991,7 +1999,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="132" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" ht="115.5">
       <c r="B32" s="4">
         <v>11</v>
       </c>
@@ -2002,11 +2010,11 @@
         <v>45602</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="8"/>
@@ -2014,7 +2022,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="99">
       <c r="B33" s="10"/>
       <c r="C33" s="5" t="s">
         <v>11</v>
@@ -2023,32 +2031,32 @@
         <v>45604</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="49.5">
       <c r="B34" s="10"/>
       <c r="C34" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -2057,10 +2065,10 @@
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="82.5">
       <c r="B35" s="4">
         <v>12</v>
       </c>
@@ -2071,21 +2079,21 @@
         <v>45609</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="82.5">
       <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
         <v>11</v>
@@ -2094,30 +2102,30 @@
         <v>45611</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="8"/>
       <c r="K36" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="82.5">
       <c r="B37" s="10"/>
       <c r="C37" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -2126,10 +2134,10 @@
       <c r="J37" s="8"/>
       <c r="K37" s="13"/>
       <c r="L37" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="33">
       <c r="B38" s="4">
         <v>13</v>
       </c>
@@ -2140,21 +2148,21 @@
         <v>45616</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="99">
       <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
         <v>11</v>
@@ -2163,7 +2171,7 @@
         <v>45618</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -2173,14 +2181,14 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="66">
       <c r="B40" s="10"/>
       <c r="C40" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -2190,7 +2198,7 @@
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="148.5">
       <c r="B41" s="4">
         <v>14</v>
       </c>
@@ -2201,23 +2209,23 @@
         <v>45623</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="G41" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="33">
       <c r="B42" s="10"/>
       <c r="C42" s="5" t="s">
         <v>11</v>
@@ -2226,30 +2234,30 @@
         <v>45625</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="8"/>
       <c r="K42" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="49.5">
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -2259,28 +2267,28 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="82.5">
       <c r="B44" s="10"/>
       <c r="C44" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="6">
         <v>45627</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K44" s="13"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="16.5">
       <c r="B45" s="4">
         <v>15</v>
       </c>
@@ -2291,7 +2299,7 @@
         <v>45630</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2301,7 +2309,7 @@
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="132" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="99">
       <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
         <v>11</v>
@@ -2310,7 +2318,7 @@
         <v>45632</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2319,49 +2327,49 @@
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="66">
       <c r="B47" s="10"/>
       <c r="C47" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K47" s="13"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="2:12" ht="165" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" ht="115.5">
       <c r="B48" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="6">
         <v>45639</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K48" s="8"/>
       <c r="L48" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved AE from Friday
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111C07BB-CBB8-4A81-84D0-878A8173BDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{111C07BB-CBB8-4A81-84D0-878A8173BDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E9324EB-51F1-4948-B346-9E2FF0D33A08}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1227,13 +1227,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>120</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="33">
+    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="66">
+    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66">
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5">
+    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="K6" s="33"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="99">
+    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="165">
+    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -1479,9 +1479,6 @@
       </c>
       <c r="G9" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
@@ -1492,7 +1489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5">
+    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -1514,13 +1511,15 @@
       <c r="G10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" ht="66">
+    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -1546,7 +1545,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="66">
+    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>5</v>
       </c>
@@ -1575,7 +1574,7 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="66">
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>11</v>
@@ -1596,7 +1595,7 @@
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" ht="66">
+    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="C14" s="24"/>
       <c r="D14" s="26"/>
@@ -1611,7 +1610,7 @@
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="9" t="s">
         <v>18</v>
@@ -1630,7 +1629,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="33">
+    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>6</v>
       </c>
@@ -1659,7 +1658,7 @@
       </c>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="2:12" ht="16.5">
+    <row r="17" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="5" t="s">
         <v>11</v>
@@ -1678,7 +1677,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="66">
+    <row r="18" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
         <v>18</v>
@@ -1695,7 +1694,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="66">
+    <row r="19" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>7</v>
       </c>
@@ -1722,7 +1721,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="66">
+    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -1747,7 +1746,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="16.5">
+    <row r="21" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" s="9" t="s">
         <v>18</v>
@@ -1768,7 +1767,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="66">
+    <row r="22" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>8</v>
       </c>
@@ -1789,7 +1788,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="2:12" ht="115.5">
+    <row r="23" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
       <c r="C23" s="5" t="s">
         <v>11</v>
@@ -1810,7 +1809,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="66">
+    <row r="24" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" s="9" t="s">
         <v>18</v>
@@ -1827,7 +1826,7 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="99">
+    <row r="25" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>9</v>
       </c>
@@ -1852,7 +1851,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="132">
+    <row r="26" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
       <c r="C26" s="5" t="s">
         <v>11</v>
@@ -1877,7 +1876,7 @@
       </c>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="49.5">
+    <row r="27" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
       <c r="C27" s="9" t="s">
         <v>18</v>
@@ -1896,7 +1895,7 @@
       <c r="K27" s="13"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="49.5">
+    <row r="28" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <v>10</v>
       </c>
@@ -1921,7 +1920,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="66">
+    <row r="29" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
         <v>11</v>
@@ -1946,7 +1945,7 @@
       </c>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="99">
+    <row r="30" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
         <v>18</v>
@@ -1965,7 +1964,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="115.5">
+    <row r="31" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <v>11</v>
       </c>
@@ -1988,7 +1987,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="99">
+    <row r="32" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="5" t="s">
         <v>11</v>
@@ -2015,7 +2014,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="49.5">
+    <row r="33" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
       <c r="C33" s="9" t="s">
         <v>18</v>
@@ -2034,7 +2033,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="82.5">
+    <row r="34" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>12</v>
       </c>
@@ -2059,7 +2058,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="82.5">
+    <row r="35" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="5" t="s">
         <v>11</v>
@@ -2084,7 +2083,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5">
+    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B36" s="10"/>
       <c r="C36" s="9" t="s">
         <v>92</v>
@@ -2103,7 +2102,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="33">
+    <row r="37" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>13</v>
       </c>
@@ -2128,7 +2127,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="99">
+    <row r="38" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>11</v>
@@ -2147,7 +2146,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="66">
+    <row r="39" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B39" s="10"/>
       <c r="C39" s="9" t="s">
         <v>18</v>
@@ -2164,7 +2163,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="148.5">
+    <row r="40" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
         <v>14</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="33">
+    <row r="41" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
         <v>11</v>
@@ -2216,7 +2215,7 @@
       </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="2:12" ht="49.5">
+    <row r="42" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
         <v>18</v>
@@ -2233,7 +2232,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="82.5">
+    <row r="43" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
         <v>108</v>
@@ -2254,7 +2253,7 @@
       <c r="K43" s="13"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="16.5">
+    <row r="44" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>15</v>
       </c>
@@ -2275,7 +2274,7 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="99">
+    <row r="45" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
       <c r="C45" s="5" t="s">
         <v>11</v>
@@ -2296,7 +2295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="66">
+    <row r="46" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B46" s="10"/>
       <c r="C46" s="9" t="s">
         <v>18</v>
@@ -2315,7 +2314,7 @@
       <c r="K46" s="13"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="115.5">
+    <row r="47" spans="2:12" ht="165" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Added model conditions ae
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{111C07BB-CBB8-4A81-84D0-878A8173BDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E9324EB-51F1-4948-B346-9E2FF0D33A08}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8901D6D-1E4B-4C52-8DC0-61AC2784FC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="147">
   <si>
     <t>week</t>
   </si>
@@ -472,13 +472,16 @@
   </si>
   <si>
     <t>/prepare/model-conditions-prep.html</t>
+  </si>
+  <si>
+    <t>/ae/05-conditions.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1227,13 +1230,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="18" t="s">
         <v>120</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="33">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="66">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1351,7 +1354,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="66">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="49.5">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="K6" s="33"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="99">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -1460,7 +1463,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="165">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -1479,6 +1482,9 @@
       </c>
       <c r="G9" s="5" t="s">
         <v>138</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
@@ -1489,7 +1495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="115.5">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -1511,15 +1517,13 @@
       <c r="G10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>141</v>
-      </c>
+      <c r="H10" s="13"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="66">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -1539,18 +1543,18 @@
       <c r="G11" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="I11" s="9"/>
       <c r="J11" s="8"/>
       <c r="K11" s="5"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B12" s="4">
-        <v>5</v>
-      </c>
+    <row r="12" spans="1:12" ht="66">
+      <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D12" s="6">
         <v>45560</v>
@@ -1574,7 +1578,7 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="66">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>11</v>
@@ -1595,7 +1599,7 @@
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="66">
       <c r="B14" s="22"/>
       <c r="C14" s="24"/>
       <c r="D14" s="26"/>
@@ -1610,7 +1614,7 @@
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="16.5">
       <c r="B15" s="10"/>
       <c r="C15" s="9" t="s">
         <v>18</v>
@@ -1629,7 +1633,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="33">
       <c r="B16" s="4">
         <v>6</v>
       </c>
@@ -1658,7 +1662,7 @@
       </c>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="16.5">
       <c r="B17" s="10"/>
       <c r="C17" s="5" t="s">
         <v>11</v>
@@ -1677,7 +1681,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="66">
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
         <v>18</v>
@@ -1694,7 +1698,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="66">
       <c r="B19" s="4">
         <v>7</v>
       </c>
@@ -1721,7 +1725,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="66">
       <c r="B20" s="10"/>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -1746,7 +1750,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="16.5">
       <c r="B21" s="10"/>
       <c r="C21" s="9" t="s">
         <v>18</v>
@@ -1767,7 +1771,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="66">
       <c r="B22" s="4">
         <v>8</v>
       </c>
@@ -1788,7 +1792,7 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="115.5">
       <c r="B23" s="10"/>
       <c r="C23" s="5" t="s">
         <v>11</v>
@@ -1809,7 +1813,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="66">
       <c r="B24" s="10"/>
       <c r="C24" s="9" t="s">
         <v>18</v>
@@ -1826,7 +1830,7 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="99">
       <c r="B25" s="4">
         <v>9</v>
       </c>
@@ -1851,7 +1855,7 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="132">
       <c r="B26" s="10"/>
       <c r="C26" s="5" t="s">
         <v>11</v>
@@ -1876,7 +1880,7 @@
       </c>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="49.5">
       <c r="B27" s="10"/>
       <c r="C27" s="9" t="s">
         <v>18</v>
@@ -1895,7 +1899,7 @@
       <c r="K27" s="13"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="49.5">
       <c r="B28" s="4">
         <v>10</v>
       </c>
@@ -1920,7 +1924,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="66">
       <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
         <v>11</v>
@@ -1945,7 +1949,7 @@
       </c>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" ht="99">
       <c r="B30" s="10"/>
       <c r="C30" s="5" t="s">
         <v>18</v>
@@ -1964,7 +1968,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" ht="115.5">
       <c r="B31" s="4">
         <v>11</v>
       </c>
@@ -1987,7 +1991,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" ht="99">
       <c r="B32" s="10"/>
       <c r="C32" s="5" t="s">
         <v>11</v>
@@ -2014,7 +2018,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="49.5">
       <c r="B33" s="10"/>
       <c r="C33" s="9" t="s">
         <v>18</v>
@@ -2033,7 +2037,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="82.5">
       <c r="B34" s="4">
         <v>12</v>
       </c>
@@ -2058,7 +2062,7 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="82.5">
       <c r="B35" s="10"/>
       <c r="C35" s="5" t="s">
         <v>11</v>
@@ -2083,7 +2087,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="82.5">
       <c r="B36" s="10"/>
       <c r="C36" s="9" t="s">
         <v>92</v>
@@ -2102,7 +2106,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="33">
       <c r="B37" s="4">
         <v>13</v>
       </c>
@@ -2127,7 +2131,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="99">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>11</v>
@@ -2146,7 +2150,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="66">
       <c r="B39" s="10"/>
       <c r="C39" s="9" t="s">
         <v>18</v>
@@ -2163,7 +2167,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="148.5">
       <c r="B40" s="4">
         <v>14</v>
       </c>
@@ -2190,7 +2194,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="33">
       <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
         <v>11</v>
@@ -2215,7 +2219,7 @@
       </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="49.5">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
         <v>18</v>
@@ -2232,7 +2236,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="82.5">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
         <v>108</v>
@@ -2253,7 +2257,7 @@
       <c r="K43" s="13"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="16.5">
       <c r="B44" s="4">
         <v>15</v>
       </c>
@@ -2274,7 +2278,7 @@
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="99">
       <c r="B45" s="10"/>
       <c r="C45" s="5" t="s">
         <v>11</v>
@@ -2295,7 +2299,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="66">
       <c r="B46" s="10"/>
       <c r="C46" s="9" t="s">
         <v>18</v>
@@ -2314,7 +2318,7 @@
       <c r="K46" s="13"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="165" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="115.5">
       <c r="B47" s="4" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Added model condition activity
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890B428F-B66F-40A9-87A9-FBFD73AB4C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2ADAD3-BCA5-4B2E-AEA0-46061421DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="147">
   <si>
     <t>week</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>/ae/ae-05-math-models.html</t>
+  </si>
+  <si>
+    <t>/ae/ae-06-conditions.html</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1231,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1547,6 +1550,9 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="66">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>15</v>
@@ -1563,7 +1569,9 @@
       <c r="G12" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="I12" s="9"/>
       <c r="J12" s="8"/>
       <c r="K12" s="9" t="s">

</xml_diff>

<commit_message>
Replaced wrong slideshow, redux
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E1DB9-1CD6-4647-84C6-15D43DBE942F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB2A02C-AE86-436D-9600-06A4C90A6B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -474,7 +474,7 @@
     <t>HW 02 Due/ HW 03 Assigned</t>
   </si>
   <si>
-    <t>/slides/09-math-models-2.html</t>
+    <t>/slides/09-slr-math-models-2.html</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Shifting outlier and transformation stuff around
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E87360A-AFF5-4D1C-A0D5-7067556386BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1EDD0-5263-4D7D-884F-33E1221BB8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="164">
   <si>
     <t>week</t>
   </si>
@@ -487,6 +487,45 @@
   </si>
   <si>
     <t>/ae/ae-07-model-eval.html</t>
+  </si>
+  <si>
+    <t>Project Introduction</t>
+  </si>
+  <si>
+    <t>Multiple linear regression</t>
+  </si>
+  <si>
+    <t>SLR: Transformations</t>
+  </si>
+  <si>
+    <t>SLR: Outliers</t>
+  </si>
+  <si>
+    <t>/prepare/transformations-prep.html</t>
+  </si>
+  <si>
+    <t>/prepare/outliers-prep.html</t>
+  </si>
+  <si>
+    <t>/prepare/introduction-prep.html</t>
+  </si>
+  <si>
+    <t>/prepare/regression-prep.html</t>
+  </si>
+  <si>
+    <t>/prepare/regression /-prep.html</t>
+  </si>
+  <si>
+    <t>/prctare/review-prct.html</t>
+  </si>
+  <si>
+    <t>/prctare/exam 01-prct.html</t>
+  </si>
+  <si>
+    <t>/slides/12-slr-transformations.html</t>
+  </si>
+  <si>
+    <t>/slides/13-slr-outliers.html</t>
   </si>
 </sst>
 </file>
@@ -593,7 +632,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -815,13 +854,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -944,6 +994,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1281,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1663,212 +1719,216 @@
       <c r="K13" s="41"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="1:12" ht="66">
-      <c r="B14" s="21"/>
-      <c r="C14" s="23" t="s">
+    <row r="14" spans="1:12" ht="49.5">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="39">
+        <v>45553</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="44"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" spans="1:12" ht="33">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="39">
+        <v>45555</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="44"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="40"/>
+    </row>
+    <row r="16" spans="1:12" ht="49.5">
+      <c r="B16" s="37">
+        <v>6</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="39">
+        <v>45558</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="40"/>
+    </row>
+    <row r="17" spans="2:12" ht="66">
+      <c r="B17" s="37"/>
+      <c r="C17" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="39">
+        <v>45560</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="40"/>
+    </row>
+    <row r="18" spans="2:12" ht="66">
+      <c r="B18" s="21"/>
+      <c r="C18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="25">
         <v>45562</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="29" t="s">
+      <c r="F18" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:12" ht="66">
-      <c r="B15" s="22"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="15" t="s">
+      <c r="H18" s="31"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="2:12" ht="66">
+      <c r="B19" s="22"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.5">
-      <c r="B16" s="10"/>
-      <c r="C16" s="9" t="s">
+      <c r="F19" s="28"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+    </row>
+    <row r="20" spans="2:12" ht="16.5">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="7" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9" t="s">
+      <c r="F20" s="8"/>
+      <c r="G20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="2:12" ht="33">
-      <c r="B17" s="4">
-        <v>6</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="6">
-        <v>45567</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="2:12" ht="16.5">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="6">
-        <v>45569</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" ht="66">
-      <c r="B19" s="10"/>
-      <c r="C19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="2:12" ht="66">
-      <c r="B20" s="4">
-        <v>7</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="6">
-        <v>45574</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="13"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:12" ht="66">
-      <c r="B21" s="10"/>
+    <row r="21" spans="2:12" ht="33">
+      <c r="B21" s="4">
+        <v>6</v>
+      </c>
       <c r="C21" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D21" s="6">
-        <v>45576</v>
+        <v>45567</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="K21" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:12" ht="16.5">
       <c r="B22" s="10"/>
-      <c r="C22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="8"/>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6">
+        <v>45569</v>
+      </c>
       <c r="E22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9" t="s">
-        <v>49</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="66">
-      <c r="B23" s="4">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="6">
-        <v>45581</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" ht="16.5">
+      <c r="B23" s="10"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -1877,133 +1937,133 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="115.5">
+    <row r="24" spans="2:12" ht="66">
       <c r="B24" s="10"/>
-      <c r="C24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="6">
-        <v>45583</v>
-      </c>
+      <c r="C24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="13"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="2:12" ht="66">
-      <c r="B25" s="10"/>
-      <c r="C25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="8"/>
+      <c r="B25" s="4">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="6">
+        <v>45574</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="13"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="99">
-      <c r="B26" s="4">
-        <v>9</v>
-      </c>
+    <row r="26" spans="2:12" ht="66">
+      <c r="B26" s="10"/>
       <c r="C26" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D26" s="6">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G26" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="132">
+    <row r="27" spans="2:12" ht="16.5">
       <c r="B27" s="10"/>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="6">
-        <v>45590</v>
-      </c>
+      <c r="C27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="2:12" ht="49.5">
-      <c r="B28" s="10"/>
-      <c r="C28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7" t="s">
-        <v>62</v>
+      <c r="K27" s="8"/>
+      <c r="L27" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="66">
+      <c r="B28" s="4">
+        <v>8</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="6">
+        <v>45581</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K28" s="13"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="49.5">
-      <c r="B29" s="4">
-        <v>10</v>
-      </c>
+    <row r="29" spans="2:12" ht="115.5">
+      <c r="B29" s="10"/>
       <c r="C29" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D29" s="6">
-        <v>45595</v>
+        <v>45583</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="G29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="13"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -2011,221 +2071,217 @@
     </row>
     <row r="30" spans="2:12" ht="66">
       <c r="B30" s="10"/>
-      <c r="C30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="6">
-        <v>45597</v>
-      </c>
+      <c r="C30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
     <row r="31" spans="2:12" ht="99">
-      <c r="B31" s="10"/>
+      <c r="B31" s="4">
+        <v>9</v>
+      </c>
       <c r="C31" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D31" s="6">
-        <v>45598</v>
+        <v>45588</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="G31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="13"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="115.5">
-      <c r="B32" s="4">
+    <row r="32" spans="2:12" ht="132">
+      <c r="B32" s="10"/>
+      <c r="C32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D32" s="6">
-        <v>45602</v>
+        <v>45590</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
+      <c r="K32" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="99">
+    <row r="33" spans="2:12" ht="49.5">
       <c r="B33" s="10"/>
-      <c r="C33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="6">
-        <v>45604</v>
-      </c>
+      <c r="C33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="8"/>
       <c r="E33" s="7" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F33" s="8"/>
-      <c r="G33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" s="8"/>
-      <c r="K33" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" s="13"/>
       <c r="L33" s="8"/>
     </row>
     <row r="34" spans="2:12" ht="49.5">
-      <c r="B34" s="10"/>
-      <c r="C34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="8"/>
+      <c r="B34" s="4">
+        <v>10</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="6">
+        <v>45595</v>
+      </c>
       <c r="E34" s="7" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
+      <c r="G34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="82.5">
-      <c r="B35" s="4">
-        <v>12</v>
-      </c>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" spans="2:12" ht="66">
+      <c r="B35" s="10"/>
       <c r="C35" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D35" s="6">
-        <v>45609</v>
+        <v>45597</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35" s="13"/>
+        <v>69</v>
+      </c>
+      <c r="I35" s="8"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="K35" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5">
+    <row r="36" spans="2:12" ht="99">
       <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45598</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="2:12" ht="115.5">
+      <c r="B37" s="4">
         <v>11</v>
       </c>
-      <c r="D36" s="6">
-        <v>45611</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" s="13"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="2:12" ht="82.5">
-      <c r="B37" s="10"/>
-      <c r="C37" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="8"/>
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="6">
+        <v>45602</v>
+      </c>
       <c r="E37" s="7" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="G37" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="13"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="33">
-      <c r="B38" s="4">
-        <v>13</v>
-      </c>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="2:12" ht="99">
+      <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D38" s="6">
-        <v>45616</v>
+        <v>45604</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="G38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="I38" s="9" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="9" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="99">
+    <row r="39" spans="2:12" ht="49.5">
       <c r="B39" s="10"/>
-      <c r="C39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="6">
-        <v>45618</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>94</v>
+      <c r="C39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -2233,127 +2289,131 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="2:12" ht="66">
-      <c r="B40" s="10"/>
-      <c r="C40" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="11" t="s">
-        <v>95</v>
+      <c r="L39" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="82.5">
+      <c r="B40" s="4">
+        <v>12</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="6">
+        <v>45609</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="G40" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="13"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="148.5">
-      <c r="B41" s="4">
-        <v>14</v>
-      </c>
+    <row r="41" spans="2:12" ht="82.5">
+      <c r="B41" s="10"/>
       <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45611</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="L41" s="8"/>
+    </row>
+    <row r="42" spans="2:12" ht="82.5">
+      <c r="B42" s="10"/>
+      <c r="C42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="33">
+      <c r="B43" s="4">
+        <v>13</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="6">
-        <v>45623</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="33">
-      <c r="B42" s="10"/>
-      <c r="C42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="6">
-        <v>45625</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42" s="13"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="2:12" ht="49.5">
-      <c r="B43" s="10"/>
-      <c r="C43" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="8"/>
+      <c r="D43" s="6">
+        <v>45616</v>
+      </c>
       <c r="E43" s="7" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="I43" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
+      <c r="K43" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="82.5">
+    <row r="44" spans="2:12" ht="99">
       <c r="B44" s="10"/>
       <c r="C44" s="5" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="D44" s="6">
-        <v>45627</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>105</v>
+        <v>45618</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K44" s="13"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="16.5">
-      <c r="B45" s="4">
-        <v>15</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="6">
-        <v>45630</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>107</v>
+    <row r="45" spans="2:12" ht="66">
+      <c r="B45" s="10"/>
+      <c r="C45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2363,66 +2423,177 @@
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="99">
-      <c r="B46" s="10"/>
+    <row r="46" spans="2:12" ht="148.5">
+      <c r="B46" s="4">
+        <v>14</v>
+      </c>
       <c r="C46" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D46" s="6">
-        <v>45632</v>
+        <v>45623</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H46" s="13"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="66">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="33">
       <c r="B47" s="10"/>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="6">
+        <v>45625</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I47" s="13"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="2:12" ht="49.5">
+      <c r="B48" s="10"/>
+      <c r="C48" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="K47" s="13"/>
-      <c r="L47" s="8"/>
-    </row>
-    <row r="48" spans="2:12" ht="115.5">
-      <c r="B48" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="6">
-        <v>45639</v>
-      </c>
+      <c r="D48" s="8"/>
       <c r="E48" s="7" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+    </row>
+    <row r="49" spans="2:12" ht="82.5">
+      <c r="B49" s="10"/>
+      <c r="C49" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="6">
+        <v>45627</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" s="13"/>
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="2:12" ht="16.5">
+      <c r="B50" s="4">
+        <v>15</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="6">
+        <v>45630</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+    </row>
+    <row r="51" spans="2:12" ht="99">
+      <c r="B51" s="10"/>
+      <c r="C51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="6">
+        <v>45632</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="66">
+      <c r="B52" s="10"/>
+      <c r="C52" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="K52" s="13"/>
+      <c r="L52" s="8"/>
+    </row>
+    <row r="53" spans="2:12" ht="115.5">
+      <c r="B53" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="6">
+        <v>45639</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="5" t="s">
+      <c r="K53" s="8"/>
+      <c r="L53" s="5" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added project to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFB2AD3-E985-48A0-8B25-607BC29FBF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA4D918-9D02-4A8A-813E-CAE306F0E2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
   <si>
     <t>week</t>
   </si>
@@ -535,13 +535,19 @@
   </si>
   <si>
     <t>/prepare/project-introduction-prep.html</t>
+  </si>
+  <si>
+    <t>HW 04 Due/HW 05 Assigned</t>
+  </si>
+  <si>
+    <t>Project Stage I Assigned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +609,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -867,7 +880,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -993,6 +1006,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1332,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1794,8 +1810,12 @@
       <c r="G16" s="39"/>
       <c r="H16" s="42"/>
       <c r="I16" s="40"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
+      <c r="J16" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="39" t="s">
+        <v>168</v>
+      </c>
       <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:12" ht="33">
@@ -1846,7 +1866,9 @@
       <c r="H18" s="29"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="K18" s="26" t="s">
+        <v>167</v>
+      </c>
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" ht="66">
@@ -2618,7 +2640,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J16" r:id="rId1" location="project-proposal" display="https://mat212fa24.netlify.app/project-instructions#project-proposal" xr:uid="{640FB934-CEF3-4FA6-8044-3AEE5553F6A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added categorical data lesson
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F1C45-F556-4EF5-8848-7EDC462124E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB2F1C45-F556-4EF5-8848-7EDC462124E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C2EB1DB-0EA7-4762-B271-89CDDB2C9D51}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
   <si>
     <t>week</t>
   </si>
@@ -550,13 +550,19 @@
   </si>
   <si>
     <t>/prepare/mlr-inference-prep.html</t>
+  </si>
+  <si>
+    <t>/slides/17-categorical-predictors.html</t>
+  </si>
+  <si>
+    <t>/ae/ae-12-categorical-predictors.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -893,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -1008,7 +1014,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1033,12 +1039,6 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1379,16 +1379,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>104</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="33">
+    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="66">
+    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66">
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5">
+    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="K6" s="28"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="99">
+    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="165">
+    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5">
+    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" ht="148.5">
+    <row r="11" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="66">
+    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="99">
+    <row r="13" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="K13" s="36"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:12" ht="66">
+    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="K14" s="36"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:12" ht="49.5">
+    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5">
+    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" ht="99">
+    <row r="17" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="K17" s="36"/>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" ht="33">
+    <row r="18" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" ht="66">
+    <row r="19" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="J19" s="24"/>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="1:12" ht="66">
+    <row r="20" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
     </row>
-    <row r="21" spans="1:12" ht="49.5">
+    <row r="21" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" ht="66">
+    <row r="22" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2011,14 +2011,18 @@
       <c r="F22" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
+      <c r="G22" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>173</v>
+      </c>
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:12" ht="33">
+    <row r="23" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -2040,7 +2044,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="16.5">
+    <row r="24" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -2064,7 +2068,7 @@
       </c>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" ht="66">
+    <row r="25" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2090,7 +2094,7 @@
       </c>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="66">
+    <row r="26" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -2112,7 +2116,7 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" ht="66">
+    <row r="27" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2134,7 +2138,7 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" ht="66">
+    <row r="28" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="5" t="s">
         <v>11</v>
@@ -2159,7 +2163,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="16.5">
+    <row r="29" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
         <v>18</v>
@@ -2180,7 +2184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="66">
+    <row r="30" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
         <v>8</v>
       </c>
@@ -2201,7 +2205,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" ht="115.5">
+    <row r="31" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
         <v>11</v>
@@ -2222,7 +2226,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="66">
+    <row r="32" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="9" t="s">
         <v>18</v>
@@ -2239,7 +2243,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="99">
+    <row r="33" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>9</v>
       </c>
@@ -2264,7 +2268,7 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="2:12" ht="132">
+    <row r="34" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
       <c r="C34" s="5" t="s">
         <v>11</v>
@@ -2289,7 +2293,7 @@
       </c>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="49.5">
+    <row r="35" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="9" t="s">
         <v>18</v>
@@ -2308,7 +2312,7 @@
       <c r="K35" s="13"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="49.5">
+    <row r="36" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
         <v>10</v>
       </c>
@@ -2333,7 +2337,7 @@
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="2:12" ht="66">
+    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B37" s="10"/>
       <c r="C37" s="5" t="s">
         <v>11</v>
@@ -2358,7 +2362,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="99">
+    <row r="38" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>18</v>
@@ -2377,7 +2381,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="115.5">
+    <row r="39" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
         <v>11</v>
       </c>
@@ -2400,7 +2404,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="99">
+    <row r="40" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B40" s="10"/>
       <c r="C40" s="5" t="s">
         <v>11</v>
@@ -2427,7 +2431,7 @@
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="49.5">
+    <row r="41" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="9" t="s">
         <v>18</v>
@@ -2446,7 +2450,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="82.5">
+    <row r="42" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
         <v>12</v>
       </c>
@@ -2471,7 +2475,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="82.5">
+    <row r="43" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
         <v>11</v>
@@ -2496,7 +2500,7 @@
       </c>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="82.5">
+    <row r="44" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B44" s="10"/>
       <c r="C44" s="9" t="s">
         <v>76</v>
@@ -2515,7 +2519,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="33">
+    <row r="45" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
         <v>13</v>
       </c>
@@ -2540,7 +2544,7 @@
       </c>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="99">
+    <row r="46" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
         <v>11</v>
@@ -2559,7 +2563,7 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="66">
+    <row r="47" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B47" s="10"/>
       <c r="C47" s="9" t="s">
         <v>18</v>
@@ -2576,7 +2580,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="2:12" ht="148.5">
+    <row r="48" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
         <v>14</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="33">
+    <row r="49" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
       <c r="C49" s="5" t="s">
         <v>11</v>
@@ -2628,7 +2632,7 @@
       </c>
       <c r="L49" s="8"/>
     </row>
-    <row r="50" spans="2:12" ht="49.5">
+    <row r="50" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
       <c r="C50" s="9" t="s">
         <v>18</v>
@@ -2645,7 +2649,7 @@
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="2:12" ht="82.5">
+    <row r="51" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="5" t="s">
         <v>92</v>
@@ -2666,7 +2670,7 @@
       <c r="K51" s="13"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="2:12" ht="16.5">
+    <row r="52" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>15</v>
       </c>
@@ -2687,7 +2691,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="2:12" ht="99">
+    <row r="53" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
       <c r="C53" s="5" t="s">
         <v>11</v>
@@ -2708,7 +2712,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="66">
+    <row r="54" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
       <c r="C54" s="9" t="s">
         <v>18</v>
@@ -2727,7 +2731,7 @@
       <c r="K54" s="13"/>
       <c r="L54" s="8"/>
     </row>
-    <row r="55" spans="2:12" ht="115.5">
+    <row r="55" spans="2:12" ht="165" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Added model comparison 1
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212FA24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{FB2F1C45-F556-4EF5-8848-7EDC462124E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28F2D5AE-9B83-42EC-A212-F5382E083D0D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE476551-B5EF-43B6-951A-2CD24A250B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="176">
   <si>
     <t>week</t>
   </si>
@@ -132,12 +132,6 @@
     <t>Exam 01</t>
   </si>
   <si>
-    <t>Lab 05</t>
-  </si>
-  <si>
-    <t>/slides/lab-05.html</t>
-  </si>
-  <si>
     <t>NO LECTURE: Fall Break</t>
   </si>
   <si>
@@ -556,13 +550,25 @@
   </si>
   <si>
     <t>/ae/ae-13-mlr-conditions.html</t>
+  </si>
+  <si>
+    <t>MLR: Model Comparison</t>
+  </si>
+  <si>
+    <t>/slides/20-comparison.html</t>
+  </si>
+  <si>
+    <t>/ae/ae-14-comparison.html</t>
+  </si>
+  <si>
+    <t>/prepare/mlr-comparison-prep.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,17 +1390,17 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1430,9 +1436,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1451,17 +1457,17 @@
         <v>13</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="33">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
@@ -1474,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
@@ -1483,12 +1489,12 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="66">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -1500,19 +1506,19 @@
         <v>45530</v>
       </c>
       <c r="E4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="66">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
@@ -1528,7 +1534,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>14</v>
@@ -1538,15 +1544,15 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="49.5">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
@@ -1556,23 +1562,23 @@
         <v>45534</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="28"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1584,12 +1590,12 @@
         <v>45537</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="99">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
@@ -1602,26 +1608,26 @@
         <v>23</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="165">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
@@ -1631,29 +1637,29 @@
         <v>45541</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
       <c r="K9" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="115.5">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
@@ -1668,10 +1674,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="8"/>
@@ -1679,9 +1685,9 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="148.5">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="5" t="s">
@@ -1691,22 +1697,22 @@
         <v>45546</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="5"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="66">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
@@ -1719,26 +1725,26 @@
         <v>28</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="I12" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="99">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" s="32">
         <v>5</v>
@@ -1750,25 +1756,25 @@
         <v>45551</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="35"/>
       <c r="K13" s="36"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="66">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="33" t="s">
@@ -1778,25 +1784,25 @@
         <v>45553</v>
       </c>
       <c r="E14" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="35"/>
       <c r="K14" s="36"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="49.5">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
@@ -1806,29 +1812,29 @@
         <v>45555</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="G15" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="H15" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="H15" s="39" t="s">
-        <v>142</v>
-      </c>
       <c r="I15" s="37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J15" s="35"/>
       <c r="K15" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="49.5">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="32">
         <v>6</v>
@@ -1840,25 +1846,25 @@
         <v>45558</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="39"/>
       <c r="I16" s="37"/>
       <c r="J16" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K16" s="36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="99">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="33" t="s">
@@ -1868,16 +1874,16 @@
         <v>45560</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="35"/>
       <c r="K17" s="36"/>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="33">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="33" t="s">
@@ -1887,29 +1893,29 @@
         <v>45562</v>
       </c>
       <c r="E18" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="G18" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="36" t="s">
-        <v>141</v>
-      </c>
       <c r="H18" s="39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="66">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" s="4">
         <v>7</v>
@@ -1921,24 +1927,24 @@
         <v>45565</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G19" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>149</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>151</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="66">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="43" t="s">
@@ -1948,25 +1954,25 @@
         <v>45567</v>
       </c>
       <c r="E20" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="45" t="s">
-        <v>156</v>
-      </c>
       <c r="G20" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
     </row>
-    <row r="21" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="49.5">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="42" t="s">
@@ -1976,29 +1982,29 @@
         <v>45569</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H21" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="66">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B22" s="4">
         <v>8</v>
@@ -2010,25 +2016,25 @@
         <v>45572</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F22" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="G22" s="26" t="s">
-        <v>167</v>
-      </c>
       <c r="H22" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="33">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
@@ -2041,22 +2047,22 @@
         <v>30</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="8"/>
       <c r="K23" s="5"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="16.5">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="5" t="s">
@@ -2074,13 +2080,13 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="66">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="4">
         <v>9</v>
@@ -2092,7 +2098,7 @@
         <v>45579</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2100,13 +2106,13 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="66">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="9" t="s">
@@ -2116,7 +2122,7 @@
         <v>45581</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2126,9 +2132,9 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="66">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
@@ -2138,7 +2144,7 @@
         <v>45583</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2148,9 +2154,9 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="49.5">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="5" t="s">
@@ -2160,42 +2166,51 @@
         <v>45586</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="66">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45588</v>
+      </c>
       <c r="E29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="8"/>
+        <v>172</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="66">
       <c r="B30" s="4">
         <v>8</v>
       </c>
@@ -2206,7 +2221,7 @@
         <v>45581</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -2216,7 +2231,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="115.5">
       <c r="B31" s="10"/>
       <c r="C31" s="5" t="s">
         <v>11</v>
@@ -2225,11 +2240,11 @@
         <v>45583</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="8"/>
@@ -2237,14 +2252,14 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="66">
       <c r="B32" s="10"/>
       <c r="C32" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -2254,7 +2269,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="99">
       <c r="B33" s="4">
         <v>9</v>
       </c>
@@ -2265,21 +2280,21 @@
         <v>45588</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="132">
       <c r="B34" s="10"/>
       <c r="C34" s="5" t="s">
         <v>11</v>
@@ -2288,42 +2303,42 @@
         <v>45590</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="49.5">
       <c r="B35" s="10"/>
       <c r="C35" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K35" s="13"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" ht="49.5">
       <c r="B36" s="4">
         <v>10</v>
       </c>
@@ -2334,21 +2349,21 @@
         <v>45595</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="66">
       <c r="B37" s="10"/>
       <c r="C37" s="5" t="s">
         <v>11</v>
@@ -2357,23 +2372,23 @@
         <v>45597</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="99">
       <c r="B38" s="10"/>
       <c r="C38" s="5" t="s">
         <v>18</v>
@@ -2382,7 +2397,7 @@
         <v>45598</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -2392,7 +2407,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="115.5">
       <c r="B39" s="4">
         <v>11</v>
       </c>
@@ -2403,11 +2418,11 @@
         <v>45602</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="8"/>
@@ -2415,7 +2430,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="99">
       <c r="B40" s="10"/>
       <c r="C40" s="5" t="s">
         <v>11</v>
@@ -2424,32 +2439,32 @@
         <v>45604</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="49.5">
       <c r="B41" s="10"/>
       <c r="C41" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -2458,10 +2473,10 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="82.5">
       <c r="B42" s="4">
         <v>12</v>
       </c>
@@ -2472,21 +2487,21 @@
         <v>45609</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="82.5">
       <c r="B43" s="10"/>
       <c r="C43" s="5" t="s">
         <v>11</v>
@@ -2495,30 +2510,30 @@
         <v>45611</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="8"/>
       <c r="K43" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="82.5">
       <c r="B44" s="10"/>
       <c r="C44" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -2527,10 +2542,10 @@
       <c r="J44" s="8"/>
       <c r="K44" s="13"/>
       <c r="L44" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="33">
       <c r="B45" s="4">
         <v>13</v>
       </c>
@@ -2541,21 +2556,21 @@
         <v>45616</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L45" s="8"/>
     </row>
-    <row r="46" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="99">
       <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
         <v>11</v>
@@ -2564,7 +2579,7 @@
         <v>45618</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2574,14 +2589,14 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="66">
       <c r="B47" s="10"/>
       <c r="C47" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -2591,7 +2606,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" ht="148.5">
       <c r="B48" s="4">
         <v>14</v>
       </c>
@@ -2602,23 +2617,23 @@
         <v>45623</v>
       </c>
       <c r="E48" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="33">
       <c r="B49" s="10"/>
       <c r="C49" s="5" t="s">
         <v>11</v>
@@ -2627,30 +2642,30 @@
         <v>45625</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="8"/>
       <c r="K49" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L49" s="8"/>
     </row>
-    <row r="50" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" ht="49.5">
       <c r="B50" s="10"/>
       <c r="C50" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -2660,28 +2675,28 @@
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" ht="82.5">
       <c r="B51" s="10"/>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D51" s="6">
         <v>45627</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K51" s="13"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" ht="16.5">
       <c r="B52" s="4">
         <v>15</v>
       </c>
@@ -2692,7 +2707,7 @@
         <v>45630</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -2702,7 +2717,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" ht="99">
       <c r="B53" s="10"/>
       <c r="C53" s="5" t="s">
         <v>11</v>
@@ -2711,7 +2726,7 @@
         <v>45632</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -2720,49 +2735,49 @@
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="66">
       <c r="B54" s="10"/>
       <c r="C54" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K54" s="13"/>
       <c r="L54" s="8"/>
     </row>
-    <row r="55" spans="2:12" ht="165" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" ht="115.5">
       <c r="B55" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="6">
         <v>45639</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K55" s="8"/>
       <c r="L55" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added second model comparison slides and act
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE476551-B5EF-43B6-951A-2CD24A250B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8C7E57-FF31-4C02-BCEB-602DAF88341F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="178">
   <si>
     <t>week</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Exam 01</t>
   </si>
   <si>
-    <t>NO LECTURE: Fall Break</t>
-  </si>
-  <si>
     <t>MLR: Model comparison + cross validation</t>
   </si>
   <si>
@@ -562,6 +559,15 @@
   </si>
   <si>
     <t>/prepare/mlr-comparison-prep.html</t>
+  </si>
+  <si>
+    <t>MLR: Model Comparison Continued</t>
+  </si>
+  <si>
+    <t>/slides/21-comparison2.html</t>
+  </si>
+  <si>
+    <t>/ae/ae-15-comparison2.html</t>
   </si>
 </sst>
 </file>
@@ -588,26 +594,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Open Sans"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Open Sans"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFB0280"/>
       <name val="Open Sans"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1390,7 +1396,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1400,7 +1406,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1438,7 +1444,7 @@
     </row>
     <row r="2" spans="1:12" ht="49.5">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1457,17 +1463,17 @@
         <v>13</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="33">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
@@ -1480,7 +1486,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
@@ -1489,12 +1495,12 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="66">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -1506,10 +1512,10 @@
         <v>45530</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -1518,7 +1524,7 @@
     </row>
     <row r="5" spans="1:12" ht="66">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
@@ -1534,7 +1540,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>14</v>
@@ -1544,7 +1550,7 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>22</v>
@@ -1552,7 +1558,7 @@
     </row>
     <row r="6" spans="1:12" ht="49.5">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
@@ -1562,14 +1568,14 @@
         <v>45534</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -1578,7 +1584,7 @@
     </row>
     <row r="7" spans="1:12" ht="16.5">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1590,12 +1596,12 @@
         <v>45537</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="99">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
@@ -1608,26 +1614,26 @@
         <v>23</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" ht="165">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
@@ -1637,21 +1643,21 @@
         <v>45541</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8"/>
       <c r="K9" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>26</v>
@@ -1659,7 +1665,7 @@
     </row>
     <row r="10" spans="1:12" ht="115.5">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
@@ -1674,10 +1680,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="8"/>
@@ -1687,7 +1693,7 @@
     </row>
     <row r="11" spans="1:12" ht="148.5">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="5" t="s">
@@ -1697,14 +1703,14 @@
         <v>45546</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="5"/>
@@ -1712,7 +1718,7 @@
     </row>
     <row r="12" spans="1:12" ht="66">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
@@ -1725,26 +1731,26 @@
         <v>28</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" ht="99">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="32">
         <v>5</v>
@@ -1756,16 +1762,16 @@
         <v>45551</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="35"/>
@@ -1774,7 +1780,7 @@
     </row>
     <row r="14" spans="1:12" ht="66">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="33" t="s">
@@ -1784,16 +1790,16 @@
         <v>45553</v>
       </c>
       <c r="E14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="35"/>
@@ -1802,7 +1808,7 @@
     </row>
     <row r="15" spans="1:12" ht="49.5">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
@@ -1812,29 +1818,29 @@
         <v>45555</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I15" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" s="35"/>
       <c r="K15" s="36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L15" s="35"/>
     </row>
     <row r="16" spans="1:12" ht="49.5">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="32">
         <v>6</v>
@@ -1846,25 +1852,25 @@
         <v>45558</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="39"/>
       <c r="I16" s="37"/>
       <c r="J16" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L16" s="35"/>
     </row>
     <row r="17" spans="1:12" ht="99">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="33" t="s">
@@ -1874,7 +1880,7 @@
         <v>45560</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="35"/>
@@ -1883,7 +1889,7 @@
     </row>
     <row r="18" spans="1:12" ht="33">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="33" t="s">
@@ -1893,29 +1899,29 @@
         <v>45562</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="66">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="4">
         <v>7</v>
@@ -1927,16 +1933,16 @@
         <v>45565</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
@@ -1944,7 +1950,7 @@
     </row>
     <row r="20" spans="1:12" ht="66">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="43" t="s">
@@ -1954,16 +1960,16 @@
         <v>45567</v>
       </c>
       <c r="E20" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>153</v>
-      </c>
       <c r="H20" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
@@ -1972,7 +1978,7 @@
     </row>
     <row r="21" spans="1:12" ht="49.5">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="42" t="s">
@@ -1982,29 +1988,29 @@
         <v>45569</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G21" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>156</v>
-      </c>
       <c r="I21" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="66">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="4">
         <v>8</v>
@@ -2016,16 +2022,16 @@
         <v>45572</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F22" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G22" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>165</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>166</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
@@ -2034,7 +2040,7 @@
     </row>
     <row r="23" spans="1:12" ht="33">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
@@ -2047,13 +2053,13 @@
         <v>30</v>
       </c>
       <c r="F23" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="26" t="s">
-        <v>168</v>
-      </c>
       <c r="H23" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="8"/>
@@ -2062,7 +2068,7 @@
     </row>
     <row r="24" spans="1:12" ht="16.5">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="5" t="s">
@@ -2080,13 +2086,13 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" ht="66">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="4">
         <v>9</v>
@@ -2098,7 +2104,7 @@
         <v>45579</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2106,13 +2112,13 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L25" s="8"/>
     </row>
     <row r="26" spans="1:12" ht="66">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="9" t="s">
@@ -2122,7 +2128,7 @@
         <v>45581</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2134,7 +2140,7 @@
     </row>
     <row r="27" spans="1:12" ht="66">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
@@ -2144,7 +2150,7 @@
         <v>45583</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2156,9 +2162,11 @@
     </row>
     <row r="28" spans="1:12" ht="49.5">
       <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="10"/>
+        <v>97</v>
+      </c>
+      <c r="B28" s="4">
+        <v>10</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>19</v>
       </c>
@@ -2166,16 +2174,16 @@
         <v>45586</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G28" s="26" t="s">
+      <c r="H28" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="8"/>
@@ -2184,7 +2192,7 @@
     </row>
     <row r="29" spans="1:12" ht="66">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
@@ -2194,38 +2202,43 @@
         <v>45588</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G29" s="26" t="s">
+      <c r="H29" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" ht="66">
-      <c r="B30" s="4">
-        <v>8</v>
-      </c>
+    <row r="30" spans="1:12" ht="99">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30" s="6">
-        <v>45581</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>32</v>
+        <v>45590</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>175</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="G30" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -2240,11 +2253,11 @@
         <v>45583</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="8"/>
@@ -2259,7 +2272,7 @@
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -2280,14 +2293,14 @@
         <v>45588</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="8"/>
@@ -2303,19 +2316,19 @@
         <v>45590</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L34" s="8"/>
     </row>
@@ -2326,14 +2339,14 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K35" s="13"/>
       <c r="L35" s="8"/>
@@ -2349,14 +2362,14 @@
         <v>45595</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2372,19 +2385,19 @@
         <v>45597</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L37" s="8"/>
     </row>
@@ -2397,7 +2410,7 @@
         <v>45598</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -2418,11 +2431,11 @@
         <v>45602</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="8"/>
@@ -2439,21 +2452,21 @@
         <v>45604</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L40" s="8"/>
     </row>
@@ -2464,7 +2477,7 @@
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -2473,7 +2486,7 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="82.5">
@@ -2487,14 +2500,14 @@
         <v>45609</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="8"/>
@@ -2510,30 +2523,30 @@
         <v>45611</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" s="8"/>
       <c r="G43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="8"/>
       <c r="K43" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L43" s="8"/>
     </row>
     <row r="44" spans="2:12" ht="82.5">
       <c r="B44" s="10"/>
       <c r="C44" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -2542,7 +2555,7 @@
       <c r="J44" s="8"/>
       <c r="K44" s="13"/>
       <c r="L44" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="33">
@@ -2556,17 +2569,17 @@
         <v>45616</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L45" s="8"/>
     </row>
@@ -2579,7 +2592,7 @@
         <v>45618</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -2596,7 +2609,7 @@
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -2617,20 +2630,20 @@
         <v>45623</v>
       </c>
       <c r="E48" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="G48" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="33">
@@ -2642,19 +2655,19 @@
         <v>45625</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H49" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="8"/>
       <c r="K49" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L49" s="8"/>
     </row>
@@ -2665,7 +2678,7 @@
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -2678,20 +2691,20 @@
     <row r="51" spans="2:12" ht="82.5">
       <c r="B51" s="10"/>
       <c r="C51" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D51" s="6">
         <v>45627</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K51" s="13"/>
       <c r="L51" s="8"/>
@@ -2707,7 +2720,7 @@
         <v>45630</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -2726,7 +2739,7 @@
         <v>45632</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -2735,7 +2748,7 @@
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="2:12" ht="66">
@@ -2745,39 +2758,39 @@
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K54" s="13"/>
       <c r="L54" s="8"/>
     </row>
     <row r="55" spans="2:12" ht="115.5">
       <c r="B55" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="6">
         <v>45639</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K55" s="8"/>
       <c r="L55" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>